<commit_message>
added function to create new bool columns
</commit_message>
<xml_diff>
--- a/Mod_3_Project_Factor_Plan.xlsx
+++ b/Mod_3_Project_Factor_Plan.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanni/repos/flatiron/dsc-3-final-project-online-ds-pt-100118/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A31B40B-4791-DB44-8080-A61E5C61203A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F547D724-A4CE-AD4A-A9F5-44049B99F4F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23660" yWindow="840" windowWidth="27020" windowHeight="26940" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
+    <workbookView xWindow="4200" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>Age</t>
   </si>
@@ -168,21 +168,9 @@
     <t>% missing</t>
   </si>
   <si>
-    <t>Create a new boolean factor: Sexual Partner Count Known</t>
-  </si>
-  <si>
-    <t>Create a new boolean factor: Age of First Sexual Intercourse Known</t>
-  </si>
-  <si>
-    <t>Create a new boolean factor: Num of Pregnancies Known</t>
-  </si>
-  <si>
     <t>leave missing values as NaN</t>
   </si>
   <si>
-    <t>Create a new boolean factor: Smokes Known</t>
-  </si>
-  <si>
     <t>Investigate, likely drop because there are so many nulls</t>
   </si>
   <si>
@@ -195,14 +183,59 @@
     <t>787 records are zero - that explains the nulls in the time factors below</t>
   </si>
   <si>
-    <t>no missing values, so convert to boolean?</t>
+    <t>Create a new boolean factor for if Num Pregnancies is known or unknown</t>
+  </si>
+  <si>
+    <t>Num of pregnancies known?</t>
+  </si>
+  <si>
+    <t>First sexual intercourse known?</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Create a new boolean factor for if f First Sexual Intercourse Known</t>
+  </si>
+  <si>
+    <t>Number of sexual partners known?</t>
+  </si>
+  <si>
+    <t>Create a new boolean factor for if Sexual Partner Count Known</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Age of patient at time of diagnosis</t>
+  </si>
+  <si>
+    <t>True if age of first sexual intercouse is known, otherwise False.</t>
+  </si>
+  <si>
+    <t>True if number of sexual partners is known, otherwise False.</t>
+  </si>
+  <si>
+    <t>True if number of pregnancies is known, otherwise False.</t>
+  </si>
+  <si>
+    <t>Patient smokes: True, False, Unknown</t>
+  </si>
+  <si>
+    <t>Is patient using hormonal contraceptives: True, False, Unknown (unclear if current and/or past)</t>
+  </si>
+  <si>
+    <t>Is patient using an IUD: True, False, Unknown (unclear if current and/or past)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -236,6 +269,47 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,6 +393,50 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8F899F-B60E-874A-A6D7-A5720CD23DE2}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,11 +763,12 @@
     <col min="1" max="1" width="37.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="13.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="61.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="61.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="63.1640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
@@ -671,8 +790,11 @@
       <c r="H1" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -695,9 +817,14 @@
       <c r="G2" s="9">
         <v>84</v>
       </c>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="H2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -711,7 +838,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="16">
-        <f t="shared" ref="E3:E37" si="0">D3/C3</f>
+        <f t="shared" ref="E3" si="0">D3/C3</f>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="F3" s="1">
@@ -720,387 +847,409 @@
       <c r="G3" s="1">
         <v>28</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="H3" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="31">
+        <v>858</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <f t="shared" ref="E4:E40" si="1">D4/C4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>0</v>
+      </c>
+      <c r="G4" s="32">
+        <v>1</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="8">
-        <v>858</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="8">
+        <v>858</v>
+      </c>
+      <c r="D5" s="9">
         <v>7</v>
       </c>
-      <c r="E4" s="17">
-        <f t="shared" si="0"/>
+      <c r="E5" s="17">
+        <f t="shared" ref="E5" si="2">D5/C5</f>
         <v>8.1585081585081581E-3</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F5" s="9">
         <v>10</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G5" s="9">
         <v>32</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="H5" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="21">
+        <v>858</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="6">
-        <v>858</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="6">
+        <v>858</v>
+      </c>
+      <c r="D7" s="1">
         <v>56</v>
       </c>
-      <c r="E5" s="16">
-        <f t="shared" si="0"/>
+      <c r="E7" s="16">
+        <f t="shared" ref="E7" si="3">D7/C7</f>
         <v>6.5268065268065265E-2</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H7" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="26">
+        <v>858</v>
+      </c>
+      <c r="D8" s="27">
+        <v>0</v>
+      </c>
+      <c r="E8" s="28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="27">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="21">
+        <v>858</v>
+      </c>
+      <c r="D9" s="22">
+        <v>13</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="1"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22">
+        <v>1</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="8">
+        <v>858</v>
+      </c>
+      <c r="D10" s="9">
+        <v>13</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="1"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>37</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="8">
+        <v>858</v>
+      </c>
+      <c r="D11" s="9">
+        <v>13</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="1"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>37</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="26">
+        <v>858</v>
+      </c>
+      <c r="D12" s="27">
+        <v>108</v>
+      </c>
+      <c r="E12" s="28">
+        <f t="shared" si="1"/>
+        <v>0.12587412587412589</v>
+      </c>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
+        <v>1</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="12">
+        <v>858</v>
+      </c>
+      <c r="D13" s="13">
+        <v>108</v>
+      </c>
+      <c r="E13" s="18">
+        <f t="shared" si="1"/>
+        <v>0.12587412587412589</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>30</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="21">
+        <v>858</v>
+      </c>
+      <c r="D14" s="22">
+        <v>17</v>
+      </c>
+      <c r="E14" s="23">
+        <f t="shared" si="1"/>
+        <v>1.9813519813519812E-2</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0</v>
+      </c>
+      <c r="G14" s="22">
+        <v>1</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="8">
+        <v>858</v>
+      </c>
+      <c r="D15" s="9">
+        <v>117</v>
+      </c>
+      <c r="E15" s="17">
+        <f t="shared" si="1"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>19</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="31">
+        <v>858</v>
+      </c>
+      <c r="D16" s="32">
+        <v>105</v>
+      </c>
+      <c r="E16" s="33">
+        <f t="shared" si="1"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="F16" s="32">
+        <v>0</v>
+      </c>
+      <c r="G16" s="32">
+        <v>1</v>
+      </c>
+      <c r="H16" s="34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="36">
+        <v>858</v>
+      </c>
+      <c r="D17" s="37">
+        <v>105</v>
+      </c>
+      <c r="E17" s="38">
+        <f t="shared" si="1"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="F17" s="37">
+        <v>0</v>
+      </c>
+      <c r="G17" s="37">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="8">
-        <v>858</v>
-      </c>
-      <c r="D6" s="9">
-        <v>13</v>
-      </c>
-      <c r="E6" s="17">
-        <f t="shared" si="0"/>
-        <v>1.5151515151515152E-2</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="8">
-        <v>858</v>
-      </c>
-      <c r="D7" s="9">
-        <v>13</v>
-      </c>
-      <c r="E7" s="17">
-        <f t="shared" si="0"/>
-        <v>1.5151515151515152E-2</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="9">
-        <v>37</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="8">
-        <v>858</v>
-      </c>
-      <c r="D8" s="9">
-        <v>13</v>
-      </c>
-      <c r="E8" s="17">
-        <f t="shared" si="0"/>
-        <v>1.5151515151515152E-2</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9">
-        <v>37</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="12">
-        <v>858</v>
-      </c>
-      <c r="D9" s="13">
-        <v>108</v>
-      </c>
-      <c r="E9" s="18">
-        <f t="shared" si="0"/>
-        <v>0.12587412587412589</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13">
-        <v>1</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="12">
-        <v>858</v>
-      </c>
-      <c r="D10" s="13">
-        <v>108</v>
-      </c>
-      <c r="E10" s="18">
-        <f t="shared" si="0"/>
-        <v>0.12587412587412589</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="13">
-        <v>30</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="8">
-        <v>858</v>
-      </c>
-      <c r="D11" s="9">
-        <v>17</v>
-      </c>
-      <c r="E11" s="17">
-        <f t="shared" si="0"/>
-        <v>1.9813519813519812E-2</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>1</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="8">
-        <v>858</v>
-      </c>
-      <c r="D12" s="9">
-        <v>117</v>
-      </c>
-      <c r="E12" s="17">
-        <f t="shared" si="0"/>
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="6">
-        <v>858</v>
-      </c>
-      <c r="D13" s="1">
-        <v>105</v>
-      </c>
-      <c r="E13" s="16">
-        <f t="shared" si="0"/>
-        <v>0.12237762237762238</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="6">
-        <v>858</v>
-      </c>
-      <c r="D14" s="1">
-        <v>105</v>
-      </c>
-      <c r="E14" s="16">
-        <f t="shared" si="0"/>
-        <v>0.12237762237762238</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>4</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="6">
-        <v>858</v>
-      </c>
-      <c r="D15" s="1">
-        <v>105</v>
-      </c>
-      <c r="E15" s="16">
-        <f t="shared" si="0"/>
-        <v>0.12237762237762238</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="6">
-        <v>858</v>
-      </c>
-      <c r="D16" s="1">
-        <v>105</v>
-      </c>
-      <c r="E16" s="16">
-        <f t="shared" si="0"/>
-        <v>0.12237762237762238</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="6">
-        <v>858</v>
-      </c>
-      <c r="D17" s="1">
-        <v>105</v>
-      </c>
-      <c r="E17" s="16">
-        <f t="shared" si="0"/>
-        <v>0.12237762237762238</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>48</v>
+      <c r="H17" s="39" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>39</v>
@@ -1112,7 +1261,7 @@
         <v>105</v>
       </c>
       <c r="E18" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F18" s="1">
@@ -1122,12 +1271,12 @@
         <v>1</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>39</v>
@@ -1139,7 +1288,7 @@
         <v>105</v>
       </c>
       <c r="E19" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F19" s="1">
@@ -1149,12 +1298,12 @@
         <v>1</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>39</v>
@@ -1166,7 +1315,7 @@
         <v>105</v>
       </c>
       <c r="E20" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F20" s="1">
@@ -1176,12 +1325,12 @@
         <v>1</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>39</v>
@@ -1193,7 +1342,7 @@
         <v>105</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F21" s="1">
@@ -1203,12 +1352,12 @@
         <v>1</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>39</v>
@@ -1220,7 +1369,7 @@
         <v>105</v>
       </c>
       <c r="E22" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F22" s="1">
@@ -1230,12 +1379,12 @@
         <v>1</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>39</v>
@@ -1247,7 +1396,7 @@
         <v>105</v>
       </c>
       <c r="E23" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F23" s="1">
@@ -1257,12 +1406,12 @@
         <v>1</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>39</v>
@@ -1274,7 +1423,7 @@
         <v>105</v>
       </c>
       <c r="E24" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F24" s="1">
@@ -1284,12 +1433,12 @@
         <v>1</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>39</v>
@@ -1301,7 +1450,7 @@
         <v>105</v>
       </c>
       <c r="E25" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F25" s="1">
@@ -1311,12 +1460,12 @@
         <v>1</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>39</v>
@@ -1328,7 +1477,7 @@
         <v>105</v>
       </c>
       <c r="E26" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12237762237762238</v>
       </c>
       <c r="F26" s="1">
@@ -1338,39 +1487,39 @@
         <v>1</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="8">
-        <v>858</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0</v>
-      </c>
-      <c r="E27" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="9">
-        <v>0</v>
-      </c>
-      <c r="G27" s="9">
-        <v>3</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>53</v>
+      <c r="A27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="6">
+        <v>858</v>
+      </c>
+      <c r="D27" s="1">
+        <v>105</v>
+      </c>
+      <c r="E27" s="16">
+        <f t="shared" si="1"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>39</v>
@@ -1379,25 +1528,25 @@
         <v>858</v>
       </c>
       <c r="D28" s="1">
-        <v>787</v>
-      </c>
-      <c r="E28" s="19">
-        <f t="shared" si="0"/>
-        <v>0.91724941724941722</v>
+        <v>105</v>
+      </c>
+      <c r="E28" s="16">
+        <f t="shared" si="1"/>
+        <v>0.12237762237762238</v>
       </c>
       <c r="F28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>22</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>39</v>
@@ -1406,25 +1555,25 @@
         <v>858</v>
       </c>
       <c r="D29" s="1">
-        <v>787</v>
-      </c>
-      <c r="E29" s="19">
-        <f t="shared" si="0"/>
-        <v>0.91724941724941722</v>
+        <v>105</v>
+      </c>
+      <c r="E29" s="16">
+        <f t="shared" si="1"/>
+        <v>0.12237762237762238</v>
       </c>
       <c r="F29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>22</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>38</v>
@@ -1436,206 +1585,287 @@
         <v>0</v>
       </c>
       <c r="E30" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F30" s="9">
         <v>0</v>
       </c>
       <c r="G30" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="6">
+        <v>858</v>
+      </c>
+      <c r="D31" s="1">
+        <v>787</v>
+      </c>
+      <c r="E31" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91724941724941722</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>22</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="6">
+        <v>858</v>
+      </c>
+      <c r="D32" s="1">
+        <v>787</v>
+      </c>
+      <c r="E32" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91724941724941722</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>22</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="8">
+        <v>858</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0</v>
+      </c>
+      <c r="G33" s="9">
+        <v>1</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="6">
-        <v>858</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="C34" s="6">
+        <v>858</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="8">
-        <v>858</v>
-      </c>
-      <c r="D32" s="9">
-        <v>0</v>
-      </c>
-      <c r="E32" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="9">
-        <v>0</v>
-      </c>
-      <c r="G32" s="9">
-        <v>1</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="C35" s="8">
+        <v>858</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>1</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="6">
-        <v>858</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
-        <v>1</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="C36" s="6">
+        <v>858</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="8">
-        <v>858</v>
-      </c>
-      <c r="D34" s="9">
-        <v>0</v>
-      </c>
-      <c r="E34" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="9">
-        <v>0</v>
-      </c>
-      <c r="G34" s="9">
-        <v>1</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="C37" s="8">
+        <v>858</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <v>1</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="6">
-        <v>858</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-      <c r="G35" s="1">
-        <v>1</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="C38" s="6">
+        <v>858</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B39" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="8">
-        <v>858</v>
-      </c>
-      <c r="D36" s="9">
-        <v>0</v>
-      </c>
-      <c r="E36" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="9">
-        <v>0</v>
-      </c>
-      <c r="G36" s="9">
-        <v>1</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="C39" s="8">
+        <v>858</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <v>1</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="6">
-        <v>858</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0</v>
-      </c>
-      <c r="E37" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1">
-        <v>1</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>54</v>
+      <c r="C40" s="6">
+        <v>858</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to .xls file
</commit_message>
<xml_diff>
--- a/Mod_3_Project_Factor_Plan.xlsx
+++ b/Mod_3_Project_Factor_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanni/repos/flatiron/dsc-3-final-project-online-ds-pt-100118/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F547D724-A4CE-AD4A-A9F5-44049B99F4F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCE49F4-81CB-D24B-8964-53C0CDFADEDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
+    <workbookView xWindow="10960" yWindow="2580" windowWidth="33600" windowHeight="20540" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,12 +159,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Hi</t>
-  </si>
-  <si>
     <t>% missing</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>Create a new boolean factor for if f First Sexual Intercourse Known</t>
-  </si>
-  <si>
     <t>Number of sexual partners known?</t>
   </si>
   <si>
@@ -229,6 +220,15 @@
   </si>
   <si>
     <t>Is patient using an IUD: True, False, Unknown (unclear if current and/or past)</t>
+  </si>
+  <si>
+    <t>Low Value</t>
+  </si>
+  <si>
+    <t>Hi Value</t>
+  </si>
+  <si>
+    <t>Create a new boolean factor for if First Sexual Intercourse Known</t>
   </si>
 </sst>
 </file>
@@ -348,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,6 +437,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,7 +756,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,19 +780,19 @@
         <v>37</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -818,10 +819,10 @@
         <v>84</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -848,15 +849,15 @@
         <v>28</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" s="31">
         <v>858</v>
@@ -875,10 +876,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -905,15 +906,15 @@
         <v>32</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="21">
         <v>858</v>
@@ -932,10 +933,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -962,16 +963,16 @@
         <v>11</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>53</v>
-      </c>
       <c r="C8" s="26">
         <v>858</v>
       </c>
@@ -989,10 +990,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -1019,10 +1020,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -1049,7 +1050,7 @@
         <v>37</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -1076,7 +1077,7 @@
         <v>37</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1103,10 +1104,10 @@
         <v>1</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1133,7 +1134,7 @@
         <v>30</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -1160,10 +1161,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -1190,7 +1191,7 @@
         <v>19</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -1217,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1244,7 +1245,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1271,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1298,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1325,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1352,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1379,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1406,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1433,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1460,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1487,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1514,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1541,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1568,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1595,7 +1596,7 @@
         <v>3</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1621,8 +1622,8 @@
       <c r="G31" s="1">
         <v>22</v>
       </c>
-      <c r="H31" s="34" t="s">
-        <v>46</v>
+      <c r="H31" s="40" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1648,8 +1649,8 @@
       <c r="G32" s="1">
         <v>22</v>
       </c>
-      <c r="H32" s="34" t="s">
-        <v>46</v>
+      <c r="H32" s="40" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1676,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1703,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1730,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1757,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1784,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1811,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1838,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -1865,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple ML models created
</commit_message>
<xml_diff>
--- a/Mod_3_Project_Factor_Plan.xlsx
+++ b/Mod_3_Project_Factor_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanni/repos/flatiron/dsc-3-final-project-online-ds-pt-100118/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CFC845-D419-314C-93CB-FA610F5FA31D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E490EA65-C649-6D47-BDCC-95A8FAB13533}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31020" yWindow="580" windowWidth="33600" windowHeight="29140" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
+    <workbookView xWindow="5700" yWindow="460" windowWidth="22940" windowHeight="20540" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="106">
   <si>
     <t>Age</t>
   </si>
@@ -346,13 +346,16 @@
   </si>
   <si>
     <t>add a new factor</t>
+  </si>
+  <si>
+    <t>92% of records had no data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -446,6 +449,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -486,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -625,16 +673,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -643,17 +694,54 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -972,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8F899F-B60E-874A-A6D7-A5720CD23DE2}">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123:E123"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107:C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2244,61 +2332,61 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="63" t="s">
+      <c r="B49" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63" t="s">
+      <c r="C49" s="68"/>
+      <c r="D49" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="60" t="s">
+      <c r="E49" s="68"/>
+      <c r="F49" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="G49" s="60"/>
+      <c r="G49" s="64"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="60" t="s">
+      <c r="B50" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="60"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="60" t="s">
+      <c r="B51" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="60"/>
-      <c r="D51" s="64" t="s">
+      <c r="C51" s="64"/>
+      <c r="D51" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="64"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="60"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="61" t="s">
+      <c r="B52" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="61" t="s">
+      <c r="C52" s="67"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="G52" s="61"/>
+      <c r="G52" s="67"/>
       <c r="H52" s="2" t="s">
         <v>47</v>
       </c>
@@ -2307,31 +2395,31 @@
       <c r="A53" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="60" t="s">
+      <c r="B53" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C53" s="60"/>
-      <c r="D53" s="64" t="s">
+      <c r="C53" s="64"/>
+      <c r="D53" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="64"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="60"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="64"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="C54" s="61"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
-      <c r="F54" s="61" t="s">
+      <c r="C54" s="67"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="61"/>
+      <c r="G54" s="67"/>
       <c r="H54" s="2" t="s">
         <v>47</v>
       </c>
@@ -2340,31 +2428,31 @@
       <c r="A55" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="60" t="s">
+      <c r="B55" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="60"/>
-      <c r="D55" s="64" t="s">
+      <c r="C55" s="64"/>
+      <c r="D55" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="E55" s="64"/>
-      <c r="F55" s="60"/>
-      <c r="G55" s="60"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="64"/>
+      <c r="G55" s="64"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="61" t="s">
+      <c r="B56" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="61" t="s">
+      <c r="C56" s="67"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="G56" s="61"/>
+      <c r="G56" s="67"/>
       <c r="H56" s="2" t="s">
         <v>47</v>
       </c>
@@ -2373,34 +2461,34 @@
       <c r="A57" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="62" t="s">
+      <c r="B57" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="62"/>
-      <c r="D57" s="64"/>
-      <c r="E57" s="64"/>
-      <c r="F57" s="60"/>
-      <c r="G57" s="60"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="65"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="64"/>
       <c r="H57" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="67" t="s">
+      <c r="B58" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C58" s="67"/>
-      <c r="D58" s="68" t="s">
+      <c r="C58" s="69"/>
+      <c r="D58" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="E58" s="68"/>
-      <c r="F58" s="67" t="s">
+      <c r="E58" s="70"/>
+      <c r="F58" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="G58" s="67"/>
+      <c r="G58" s="69"/>
       <c r="H58" s="10" t="s">
         <v>98</v>
       </c>
@@ -2409,14 +2497,14 @@
       <c r="A59" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="62" t="s">
+      <c r="B59" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="62"/>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="64"/>
       <c r="H59" s="2" t="s">
         <v>100</v>
       </c>
@@ -2425,14 +2513,14 @@
       <c r="A60" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="62" t="s">
+      <c r="B60" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="62"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="60"/>
-      <c r="G60" s="60"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="65"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="64"/>
       <c r="H60" s="2" t="s">
         <v>100</v>
       </c>
@@ -2441,33 +2529,33 @@
       <c r="A61" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="60" t="s">
+      <c r="B61" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="C61" s="60"/>
-      <c r="D61" s="64" t="s">
+      <c r="C61" s="64"/>
+      <c r="D61" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="64"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="60"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="64"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="66" t="s">
+      <c r="A62" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="67" t="s">
+      <c r="B62" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="67"/>
-      <c r="D62" s="68" t="s">
+      <c r="C62" s="69"/>
+      <c r="D62" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="68"/>
-      <c r="F62" s="67" t="s">
+      <c r="E62" s="70"/>
+      <c r="F62" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="G62" s="67"/>
+      <c r="G62" s="69"/>
       <c r="H62" s="10" t="s">
         <v>98</v>
       </c>
@@ -2476,46 +2564,46 @@
       <c r="A63" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="64" t="s">
+      <c r="B63" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="60"/>
-      <c r="G63" s="60"/>
+      <c r="C63" s="65"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="60" t="s">
+      <c r="B64" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="60"/>
-      <c r="D64" s="64" t="s">
+      <c r="C64" s="64"/>
+      <c r="D64" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E64" s="64"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="60"/>
+      <c r="E64" s="65"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="66" t="s">
+      <c r="A65" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="B65" s="67" t="s">
+      <c r="B65" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C65" s="67"/>
-      <c r="D65" s="68" t="s">
+      <c r="C65" s="69"/>
+      <c r="D65" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="E65" s="68"/>
-      <c r="F65" s="67" t="s">
+      <c r="E65" s="70"/>
+      <c r="F65" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="G65" s="67"/>
+      <c r="G65" s="69"/>
       <c r="H65" s="10" t="s">
         <v>98</v>
       </c>
@@ -2524,46 +2612,46 @@
       <c r="A66" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="64" t="s">
+      <c r="B66" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
-      <c r="E66" s="64"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
+      <c r="C66" s="65"/>
+      <c r="D66" s="65"/>
+      <c r="E66" s="65"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="64"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B67" s="60" t="s">
+      <c r="B67" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="60"/>
-      <c r="D67" s="64" t="s">
+      <c r="C67" s="64"/>
+      <c r="D67" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E67" s="64"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
+      <c r="E67" s="65"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="66" t="s">
+      <c r="A68" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="67" t="s">
+      <c r="B68" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="C68" s="67"/>
-      <c r="D68" s="68" t="s">
+      <c r="C68" s="69"/>
+      <c r="D68" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="E68" s="68"/>
-      <c r="F68" s="67" t="s">
+      <c r="E68" s="70"/>
+      <c r="F68" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="G68" s="67"/>
+      <c r="G68" s="69"/>
       <c r="H68" s="10" t="s">
         <v>98</v>
       </c>
@@ -2572,16 +2660,16 @@
       <c r="A69" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="62" t="s">
+      <c r="B69" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C69" s="62"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="60"/>
-      <c r="F69" s="65" t="s">
+      <c r="C69" s="63"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="G69" s="65"/>
+      <c r="G69" s="66"/>
       <c r="H69" s="2" t="s">
         <v>102</v>
       </c>
@@ -2591,14 +2679,14 @@
       <c r="A70" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="62" t="s">
+      <c r="B70" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="62"/>
-      <c r="D70" s="60"/>
-      <c r="E70" s="60"/>
-      <c r="F70" s="65"/>
-      <c r="G70" s="65"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
       <c r="H70" s="2" t="s">
         <v>103</v>
       </c>
@@ -2607,95 +2695,95 @@
       <c r="A71" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B71" s="62" t="s">
+      <c r="B71" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="62"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="60"/>
-      <c r="F71" s="65"/>
-      <c r="G71" s="65"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="62" t="s">
+      <c r="B72" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="62"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="62" t="s">
+      <c r="B73" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="62"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B74" s="62" t="s">
+      <c r="B74" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C74" s="62"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="65"/>
-      <c r="G74" s="65"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="66"/>
       <c r="H74" s="57"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B75" s="62" t="s">
+      <c r="B75" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="62"/>
-      <c r="D75" s="60"/>
-      <c r="E75" s="60"/>
-      <c r="F75" s="65"/>
-      <c r="G75" s="65"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="66"/>
       <c r="H75" s="57"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B76" s="62" t="s">
+      <c r="B76" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="62"/>
-      <c r="D76" s="60"/>
-      <c r="E76" s="60"/>
-      <c r="F76" s="65"/>
-      <c r="G76" s="65"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="64"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="66"/>
       <c r="H76" s="57"/>
     </row>
     <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B77" s="62" t="s">
+      <c r="B77" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C77" s="62"/>
-      <c r="D77" s="60"/>
-      <c r="E77" s="60"/>
-      <c r="F77" s="65"/>
-      <c r="G77" s="65"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="66"/>
       <c r="H77" s="57" t="s">
         <v>96</v>
       </c>
@@ -2704,14 +2792,14 @@
       <c r="A78" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B78" s="62" t="s">
+      <c r="B78" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C78" s="62"/>
-      <c r="D78" s="60"/>
-      <c r="E78" s="60"/>
-      <c r="F78" s="65"/>
-      <c r="G78" s="65"/>
+      <c r="C78" s="63"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="64"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="66"/>
       <c r="H78" s="57" t="s">
         <v>87</v>
       </c>
@@ -2720,14 +2808,14 @@
       <c r="A79" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B79" s="62" t="s">
+      <c r="B79" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C79" s="62"/>
-      <c r="D79" s="60"/>
-      <c r="E79" s="60"/>
-      <c r="F79" s="65"/>
-      <c r="G79" s="65"/>
+      <c r="C79" s="63"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="66"/>
       <c r="H79" s="57" t="s">
         <v>88</v>
       </c>
@@ -2736,14 +2824,14 @@
       <c r="A80" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B80" s="62" t="s">
+      <c r="B80" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="62"/>
-      <c r="D80" s="60"/>
-      <c r="E80" s="60"/>
-      <c r="F80" s="65"/>
-      <c r="G80" s="65"/>
+      <c r="C80" s="63"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="66"/>
+      <c r="G80" s="66"/>
       <c r="H80" s="57" t="s">
         <v>89</v>
       </c>
@@ -2752,150 +2840,150 @@
       <c r="A81" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B81" s="62" t="s">
+      <c r="B81" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="62"/>
-      <c r="D81" s="60"/>
-      <c r="E81" s="60"/>
-      <c r="F81" s="65"/>
-      <c r="G81" s="65"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="66"/>
+      <c r="G81" s="66"/>
       <c r="H81" s="57"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B82" s="60" t="s">
+      <c r="B82" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="60"/>
-      <c r="D82" s="60"/>
-      <c r="E82" s="60"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
       <c r="F82" s="52"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B83" s="64" t="s">
+      <c r="B83" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="C83" s="64"/>
-      <c r="D83" s="60"/>
-      <c r="E83" s="60"/>
+      <c r="C83" s="65"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
       <c r="F83" s="52"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B84" s="64" t="s">
+      <c r="B84" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="C84" s="64"/>
-      <c r="D84" s="60"/>
-      <c r="E84" s="60"/>
+      <c r="C84" s="65"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
       <c r="F84" s="52"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B85" s="60" t="s">
+      <c r="B85" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C85" s="60"/>
-      <c r="D85" s="64"/>
-      <c r="E85" s="64"/>
+      <c r="C85" s="64"/>
+      <c r="D85" s="65"/>
+      <c r="E85" s="65"/>
       <c r="F85" s="52"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B86" s="60" t="s">
+      <c r="B86" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C86" s="60"/>
-      <c r="D86" s="64"/>
-      <c r="E86" s="64"/>
+      <c r="C86" s="64"/>
+      <c r="D86" s="65"/>
+      <c r="E86" s="65"/>
       <c r="F86" s="52"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B87" s="60" t="s">
+      <c r="B87" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C87" s="60"/>
-      <c r="D87" s="64"/>
-      <c r="E87" s="64"/>
+      <c r="C87" s="64"/>
+      <c r="D87" s="65"/>
+      <c r="E87" s="65"/>
       <c r="F87" s="52"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B88" s="60" t="s">
+      <c r="B88" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C88" s="60"/>
-      <c r="D88" s="64"/>
-      <c r="E88" s="64"/>
+      <c r="C88" s="64"/>
+      <c r="D88" s="65"/>
+      <c r="E88" s="65"/>
       <c r="F88" s="52"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B89" s="60" t="s">
+      <c r="B89" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C89" s="60"/>
-      <c r="D89" s="64"/>
-      <c r="E89" s="64"/>
+      <c r="C89" s="64"/>
+      <c r="D89" s="65"/>
+      <c r="E89" s="65"/>
       <c r="F89" s="52"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B90" s="60" t="s">
+      <c r="B90" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C90" s="60"/>
-      <c r="D90" s="64"/>
-      <c r="E90" s="64"/>
+      <c r="C90" s="64"/>
+      <c r="D90" s="65"/>
+      <c r="E90" s="65"/>
       <c r="F90" s="52"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B91" s="60" t="s">
+      <c r="B91" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C91" s="60"/>
-      <c r="D91" s="64"/>
-      <c r="E91" s="64"/>
+      <c r="C91" s="64"/>
+      <c r="D91" s="65"/>
+      <c r="E91" s="65"/>
       <c r="F91" s="52"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B92" s="62" t="s">
+      <c r="B92" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="C92" s="62"/>
-      <c r="D92" s="62"/>
-      <c r="E92" s="62"/>
-      <c r="F92" s="62" t="s">
+      <c r="C92" s="63"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="63"/>
+      <c r="F92" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="G92" s="62"/>
+      <c r="G92" s="63"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="55"/>
@@ -2907,483 +2995,492 @@
       <c r="A95" s="53"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B96" s="63" t="s">
+      <c r="B96" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="63"/>
-      <c r="D96" s="63" t="s">
+      <c r="C96" s="68"/>
+      <c r="D96" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="E96" s="63"/>
-      <c r="F96" s="60" t="s">
+      <c r="E96" s="68"/>
+      <c r="F96" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="G96" s="60"/>
+      <c r="G96" s="64"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B97" s="60" t="s">
+      <c r="B97" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C97" s="60"/>
-      <c r="D97" s="60"/>
-      <c r="E97" s="60"/>
-      <c r="F97" s="60"/>
-      <c r="G97" s="60"/>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
+      <c r="F97" s="64"/>
+      <c r="G97" s="64"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="53" t="s">
+      <c r="A98" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B98" s="60" t="s">
+      <c r="B98" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C98" s="60"/>
-      <c r="D98" s="64" t="s">
+      <c r="C98" s="74"/>
+      <c r="D98" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="E98" s="64"/>
-      <c r="F98" s="60"/>
-      <c r="G98" s="60"/>
+      <c r="E98" s="72"/>
+      <c r="F98" s="64"/>
+      <c r="G98" s="64"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="54" t="s">
+      <c r="A99" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="B99" s="61" t="s">
+      <c r="B99" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="C99" s="61"/>
-      <c r="D99" s="64"/>
-      <c r="E99" s="64"/>
-      <c r="F99" s="61" t="s">
+      <c r="C99" s="82"/>
+      <c r="D99" s="83"/>
+      <c r="E99" s="83"/>
+      <c r="F99" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="G99" s="61"/>
+      <c r="G99" s="82"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="53" t="s">
+      <c r="A100" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="60" t="s">
+      <c r="B100" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C100" s="60"/>
-      <c r="D100" s="64" t="s">
+      <c r="C100" s="74"/>
+      <c r="D100" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="E100" s="64"/>
-      <c r="F100" s="60"/>
-      <c r="G100" s="60"/>
+      <c r="E100" s="72"/>
+      <c r="F100" s="64"/>
+      <c r="G100" s="64"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="54" t="s">
+      <c r="A101" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="B101" s="61" t="s">
+      <c r="B101" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="C101" s="61"/>
-      <c r="D101" s="64"/>
-      <c r="E101" s="64"/>
-      <c r="F101" s="61" t="s">
+      <c r="C101" s="82"/>
+      <c r="D101" s="83"/>
+      <c r="E101" s="83"/>
+      <c r="F101" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="G101" s="61"/>
+      <c r="G101" s="82"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="53" t="s">
+      <c r="A102" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="60" t="s">
+      <c r="B102" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C102" s="60"/>
-      <c r="D102" s="64" t="s">
+      <c r="C102" s="74"/>
+      <c r="D102" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="E102" s="64"/>
-      <c r="F102" s="60"/>
-      <c r="G102" s="60"/>
+      <c r="E102" s="72"/>
+      <c r="F102" s="64"/>
+      <c r="G102" s="64"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="54" t="s">
+      <c r="A103" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B103" s="61" t="s">
+      <c r="B103" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="61"/>
-      <c r="D103" s="64"/>
-      <c r="E103" s="64"/>
-      <c r="F103" s="61" t="s">
+      <c r="C103" s="82"/>
+      <c r="D103" s="83"/>
+      <c r="E103" s="83"/>
+      <c r="F103" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="G103" s="61"/>
+      <c r="G103" s="82"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="53" t="s">
+      <c r="A104" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="64"/>
-      <c r="C104" s="64"/>
-      <c r="D104" s="64" t="s">
+      <c r="B104" s="76"/>
+      <c r="C104" s="76"/>
+      <c r="D104" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E104" s="64"/>
-      <c r="F104" s="60"/>
-      <c r="G104" s="60"/>
-      <c r="H104" s="2" t="s">
+      <c r="E104" s="76"/>
+      <c r="F104" s="77"/>
+      <c r="G104" s="77"/>
+      <c r="H104" s="78" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="53" t="s">
+      <c r="A105" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B105" s="64"/>
-      <c r="C105" s="64"/>
-      <c r="D105" s="64" t="s">
+      <c r="B105" s="76"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E105" s="64"/>
-      <c r="F105" s="60"/>
-      <c r="G105" s="60"/>
-      <c r="H105" s="2" t="s">
+      <c r="E105" s="76"/>
+      <c r="F105" s="77"/>
+      <c r="G105" s="77"/>
+      <c r="H105" s="78" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="53" t="s">
+      <c r="A106" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="64"/>
-      <c r="C106" s="64"/>
-      <c r="D106" s="64" t="s">
+      <c r="B106" s="76"/>
+      <c r="C106" s="76"/>
+      <c r="D106" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E106" s="64"/>
-      <c r="F106" s="60"/>
-      <c r="G106" s="60"/>
-      <c r="H106" s="2" t="s">
+      <c r="E106" s="76"/>
+      <c r="F106" s="77"/>
+      <c r="G106" s="77"/>
+      <c r="H106" s="78" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="69" t="s">
+      <c r="A107" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B107" s="64" t="s">
+      <c r="B107" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="C107" s="64"/>
-      <c r="D107" s="64" t="s">
+      <c r="C107" s="65"/>
+      <c r="D107" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E107" s="64"/>
-      <c r="F107" s="60"/>
-      <c r="G107" s="60"/>
+      <c r="E107" s="65"/>
+      <c r="F107" s="64"/>
+      <c r="G107" s="64"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="69" t="s">
+      <c r="A108" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="64"/>
-      <c r="C108" s="64"/>
-      <c r="D108" s="64" t="s">
+      <c r="B108" s="72"/>
+      <c r="C108" s="72"/>
+      <c r="D108" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="E108" s="64"/>
-      <c r="F108" s="60"/>
-      <c r="G108" s="60"/>
+      <c r="E108" s="72"/>
+      <c r="F108" s="64"/>
+      <c r="G108" s="64"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="69" t="s">
+      <c r="A109" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="64" t="s">
+      <c r="B109" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="C109" s="64"/>
-      <c r="D109" s="64" t="s">
+      <c r="C109" s="65"/>
+      <c r="D109" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E109" s="64"/>
-      <c r="F109" s="60"/>
-      <c r="G109" s="60"/>
+      <c r="E109" s="65"/>
+      <c r="F109" s="64"/>
+      <c r="G109" s="64"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="69" t="s">
+      <c r="A110" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="64"/>
-      <c r="C110" s="64"/>
-      <c r="D110" s="64" t="s">
+      <c r="B110" s="72"/>
+      <c r="C110" s="72"/>
+      <c r="D110" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="E110" s="64"/>
-      <c r="F110" s="60"/>
-      <c r="G110" s="60"/>
+      <c r="E110" s="72"/>
+      <c r="F110" s="64"/>
+      <c r="G110" s="64"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="69" t="s">
+      <c r="A111" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="64" t="s">
+      <c r="B111" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="C111" s="64"/>
-      <c r="D111" s="64" t="s">
+      <c r="C111" s="65"/>
+      <c r="D111" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E111" s="64"/>
-      <c r="F111" s="60"/>
-      <c r="G111" s="60"/>
+      <c r="E111" s="65"/>
+      <c r="F111" s="64"/>
+      <c r="G111" s="64"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="53" t="s">
+      <c r="A112" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="64"/>
-      <c r="C112" s="64"/>
-      <c r="D112" s="64" t="s">
+      <c r="B112" s="76"/>
+      <c r="C112" s="76"/>
+      <c r="D112" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E112" s="64"/>
-      <c r="F112" s="65" t="s">
+      <c r="E112" s="76"/>
+      <c r="F112" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="G112" s="65"/>
-      <c r="H112" s="2" t="s">
+      <c r="G112" s="66"/>
+      <c r="H112" s="78" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="53" t="s">
+      <c r="A113" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="B113" s="64"/>
-      <c r="C113" s="64"/>
-      <c r="D113" s="64" t="s">
+      <c r="B113" s="76"/>
+      <c r="C113" s="76"/>
+      <c r="D113" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E113" s="64"/>
-      <c r="F113" s="65"/>
-      <c r="G113" s="65"/>
-      <c r="H113" s="2" t="s">
+      <c r="E113" s="76"/>
+      <c r="F113" s="66"/>
+      <c r="G113" s="66"/>
+      <c r="H113" s="78" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="53" t="s">
+      <c r="A114" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B114" s="64" t="s">
+      <c r="B114" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="C114" s="64"/>
-      <c r="D114" s="64"/>
-      <c r="E114" s="64"/>
-      <c r="F114" s="65"/>
-      <c r="G114" s="65"/>
+      <c r="C114" s="79"/>
+      <c r="D114" s="79"/>
+      <c r="E114" s="79"/>
+      <c r="F114" s="66"/>
+      <c r="G114" s="66"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="53" t="s">
+      <c r="A115" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B115" s="64"/>
-      <c r="C115" s="64"/>
-      <c r="D115" s="64" t="s">
+      <c r="B115" s="76"/>
+      <c r="C115" s="76"/>
+      <c r="D115" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E115" s="64"/>
-      <c r="F115" s="65"/>
-      <c r="G115" s="65"/>
+      <c r="E115" s="76"/>
+      <c r="F115" s="66"/>
+      <c r="G115" s="66"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="53" t="s">
+      <c r="A116" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B116" s="64"/>
-      <c r="C116" s="64"/>
-      <c r="D116" s="64" t="s">
+      <c r="B116" s="76"/>
+      <c r="C116" s="76"/>
+      <c r="D116" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E116" s="64"/>
-      <c r="F116" s="65"/>
-      <c r="G116" s="65"/>
+      <c r="E116" s="76"/>
+      <c r="F116" s="66"/>
+      <c r="G116" s="66"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="53" t="s">
+      <c r="A117" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="B117" s="64"/>
-      <c r="C117" s="64"/>
-      <c r="D117" s="64" t="s">
+      <c r="B117" s="76"/>
+      <c r="C117" s="76"/>
+      <c r="D117" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E117" s="64"/>
-      <c r="F117" s="65"/>
-      <c r="G117" s="65"/>
+      <c r="E117" s="76"/>
+      <c r="F117" s="66"/>
+      <c r="G117" s="66"/>
       <c r="H117" s="57"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="53" t="s">
+      <c r="A118" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B118" s="64"/>
-      <c r="C118" s="64"/>
-      <c r="D118" s="64" t="s">
+      <c r="B118" s="76"/>
+      <c r="C118" s="76"/>
+      <c r="D118" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E118" s="64"/>
-      <c r="F118" s="65"/>
-      <c r="G118" s="65"/>
+      <c r="E118" s="76"/>
+      <c r="F118" s="66"/>
+      <c r="G118" s="66"/>
       <c r="H118" s="57"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="53" t="s">
+      <c r="A119" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="B119" s="64"/>
-      <c r="C119" s="64"/>
-      <c r="D119" s="64" t="s">
+      <c r="B119" s="76"/>
+      <c r="C119" s="76"/>
+      <c r="D119" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E119" s="64"/>
-      <c r="F119" s="65"/>
-      <c r="G119" s="65"/>
+      <c r="E119" s="76"/>
+      <c r="F119" s="66"/>
+      <c r="G119" s="66"/>
       <c r="H119" s="57"/>
     </row>
     <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="53" t="s">
+      <c r="A120" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B120" s="64"/>
-      <c r="C120" s="64"/>
-      <c r="D120" s="64" t="s">
+      <c r="B120" s="76"/>
+      <c r="C120" s="76"/>
+      <c r="D120" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E120" s="64"/>
-      <c r="F120" s="65"/>
-      <c r="G120" s="65"/>
+      <c r="E120" s="76"/>
+      <c r="F120" s="66"/>
+      <c r="G120" s="66"/>
       <c r="H120" s="57" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="53" t="s">
+      <c r="A121" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B121" s="64" t="s">
+      <c r="B121" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="C121" s="64"/>
-      <c r="D121" s="64"/>
-      <c r="E121" s="64"/>
-      <c r="F121" s="65"/>
-      <c r="G121" s="65"/>
+      <c r="C121" s="79"/>
+      <c r="D121" s="79"/>
+      <c r="E121" s="79"/>
+      <c r="F121" s="66"/>
+      <c r="G121" s="66"/>
       <c r="H121" s="57" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="53" t="s">
+      <c r="A122" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="B122" s="64"/>
-      <c r="C122" s="64"/>
-      <c r="D122" s="64" t="s">
+      <c r="B122" s="76"/>
+      <c r="C122" s="76"/>
+      <c r="D122" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E122" s="64"/>
-      <c r="F122" s="65"/>
-      <c r="G122" s="65"/>
+      <c r="E122" s="76"/>
+      <c r="F122" s="66"/>
+      <c r="G122" s="66"/>
       <c r="H122" s="57" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="53" t="s">
+      <c r="A123" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="B123" s="64"/>
-      <c r="C123" s="64"/>
-      <c r="D123" s="64" t="s">
+      <c r="B123" s="76"/>
+      <c r="C123" s="76"/>
+      <c r="D123" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E123" s="64"/>
-      <c r="F123" s="65"/>
-      <c r="G123" s="65"/>
+      <c r="E123" s="76"/>
+      <c r="F123" s="66"/>
+      <c r="G123" s="66"/>
       <c r="H123" s="57" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A124" s="53" t="s">
+      <c r="A124" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="B124" s="64"/>
-      <c r="C124" s="64"/>
-      <c r="D124" s="64" t="s">
+      <c r="B124" s="76"/>
+      <c r="C124" s="76"/>
+      <c r="D124" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E124" s="64"/>
-      <c r="F124" s="65"/>
-      <c r="G124" s="65"/>
+      <c r="E124" s="76"/>
+      <c r="F124" s="66"/>
+      <c r="G124" s="66"/>
       <c r="H124" s="57"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A125" s="53" t="s">
+    <row r="125" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B125" s="60" t="s">
+      <c r="B125" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="C125" s="60"/>
-      <c r="D125" s="60"/>
-      <c r="E125" s="60"/>
-      <c r="F125" s="52"/>
-      <c r="G125" s="59"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A126" s="53" t="s">
+      <c r="C125" s="67"/>
+      <c r="D125" s="67"/>
+      <c r="E125" s="67"/>
+      <c r="F125" s="51"/>
+      <c r="G125" s="60"/>
+      <c r="H125" s="80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B126" s="64" t="s">
+      <c r="B126" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="C126" s="64"/>
-      <c r="D126" s="60"/>
-      <c r="E126" s="60"/>
-      <c r="F126" s="52"/>
-      <c r="G126" s="59"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A127" s="53" t="s">
+      <c r="C126" s="79"/>
+      <c r="D126" s="67"/>
+      <c r="E126" s="67"/>
+      <c r="F126" s="51"/>
+      <c r="G126" s="60"/>
+      <c r="H126" s="80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B127" s="64" t="s">
+      <c r="B127" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="C127" s="64"/>
-      <c r="D127" s="60"/>
-      <c r="E127" s="60"/>
-      <c r="F127" s="52"/>
-      <c r="G127" s="59"/>
+      <c r="C127" s="79"/>
+      <c r="D127" s="67"/>
+      <c r="E127" s="67"/>
+      <c r="F127" s="51"/>
+      <c r="G127" s="60"/>
+      <c r="H127" s="80" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B128" s="60" t="s">
+      <c r="B128" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C128" s="60"/>
-      <c r="D128" s="64"/>
-      <c r="E128" s="64"/>
+      <c r="C128" s="64"/>
+      <c r="D128" s="65"/>
+      <c r="E128" s="65"/>
       <c r="F128" s="52"/>
       <c r="G128" s="59"/>
     </row>
@@ -3391,12 +3488,12 @@
       <c r="A129" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B129" s="60" t="s">
+      <c r="B129" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C129" s="60"/>
-      <c r="D129" s="64"/>
-      <c r="E129" s="64"/>
+      <c r="C129" s="64"/>
+      <c r="D129" s="65"/>
+      <c r="E129" s="65"/>
       <c r="F129" s="52"/>
       <c r="G129" s="59"/>
     </row>
@@ -3404,12 +3501,12 @@
       <c r="A130" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B130" s="60" t="s">
+      <c r="B130" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C130" s="60"/>
-      <c r="D130" s="64"/>
-      <c r="E130" s="64"/>
+      <c r="C130" s="64"/>
+      <c r="D130" s="65"/>
+      <c r="E130" s="65"/>
       <c r="F130" s="52"/>
       <c r="G130" s="59"/>
     </row>
@@ -3417,12 +3514,12 @@
       <c r="A131" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B131" s="60" t="s">
+      <c r="B131" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C131" s="60"/>
-      <c r="D131" s="64"/>
-      <c r="E131" s="64"/>
+      <c r="C131" s="64"/>
+      <c r="D131" s="65"/>
+      <c r="E131" s="65"/>
       <c r="F131" s="52"/>
       <c r="G131" s="59"/>
     </row>
@@ -3430,12 +3527,12 @@
       <c r="A132" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B132" s="60" t="s">
+      <c r="B132" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C132" s="60"/>
-      <c r="D132" s="64"/>
-      <c r="E132" s="64"/>
+      <c r="C132" s="64"/>
+      <c r="D132" s="65"/>
+      <c r="E132" s="65"/>
       <c r="F132" s="52"/>
       <c r="G132" s="59"/>
     </row>
@@ -3443,12 +3540,12 @@
       <c r="A133" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B133" s="60" t="s">
+      <c r="B133" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C133" s="60"/>
-      <c r="D133" s="64"/>
-      <c r="E133" s="64"/>
+      <c r="C133" s="64"/>
+      <c r="D133" s="65"/>
+      <c r="E133" s="65"/>
       <c r="F133" s="52"/>
       <c r="G133" s="59"/>
     </row>
@@ -3456,12 +3553,12 @@
       <c r="A134" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B134" s="60" t="s">
+      <c r="B134" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C134" s="60"/>
-      <c r="D134" s="64"/>
-      <c r="E134" s="64"/>
+      <c r="C134" s="64"/>
+      <c r="D134" s="65"/>
+      <c r="E134" s="65"/>
       <c r="F134" s="52"/>
       <c r="G134" s="59"/>
     </row>
@@ -3469,117 +3566,105 @@
       <c r="A135" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B135" s="62" t="s">
+      <c r="B135" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="C135" s="62"/>
-      <c r="D135" s="62"/>
-      <c r="E135" s="62"/>
-      <c r="F135" s="62" t="s">
+      <c r="C135" s="63"/>
+      <c r="D135" s="63"/>
+      <c r="E135" s="63"/>
+      <c r="F135" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="G135" s="62"/>
+      <c r="G135" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="208">
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="F135:G135"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="F111:G111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="F112:G124"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="F109:G109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="F110:G110"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="F107:G107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="F106:G106"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="F104:G104"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="F97:G97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
     <mergeCell ref="F92:G92"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="D73:E73"/>
@@ -3604,92 +3689,104 @@
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D86:E86"/>
     <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="F97:G97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="F106:G106"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="F104:G104"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="F109:G109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="F107:G107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="F111:G111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="F112:G124"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="F135:G135"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:E134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wip on notebook cleanup
</commit_message>
<xml_diff>
--- a/Mod_3_Project_Factor_Plan.xlsx
+++ b/Mod_3_Project_Factor_Plan.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanni/repos/flatiron/dsc-3-final-project-online-ds-pt-100118/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E9D287-71ED-3F44-BF5C-85CC8E7AC475}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F2441B-C466-C643-BE46-E12AA13E20BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="4520" windowWidth="38900" windowHeight="21660" activeTab="1" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
+    <workbookView xWindow="11420" yWindow="4340" windowWidth="38900" windowHeight="21660" activeTab="2" xr2:uid="{077C2CD1-CFC2-6747-974C-91CE457A5D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="factors" sheetId="2" r:id="rId2"/>
+    <sheet name="factors list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="110">
   <si>
     <t>Age</t>
   </si>
@@ -562,7 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -732,128 +733,134 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2445,61 +2452,61 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="75" t="s">
+      <c r="B49" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75" t="s">
+      <c r="C49" s="116"/>
+      <c r="D49" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="75"/>
-      <c r="F49" s="72" t="s">
+      <c r="E49" s="116"/>
+      <c r="F49" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="G49" s="72"/>
+      <c r="G49" s="106"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="72"/>
-      <c r="F50" s="72"/>
-      <c r="G50" s="72"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="106"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="106"/>
+      <c r="G50" s="106"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="72" t="s">
+      <c r="B51" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="72"/>
-      <c r="D51" s="74" t="s">
+      <c r="C51" s="106"/>
+      <c r="D51" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="74"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="72"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="106"/>
+      <c r="G51" s="106"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="71" t="s">
+      <c r="B52" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="71"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="71" t="s">
+      <c r="C52" s="105"/>
+      <c r="D52" s="107"/>
+      <c r="E52" s="107"/>
+      <c r="F52" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="G52" s="71"/>
+      <c r="G52" s="105"/>
       <c r="H52" s="2" t="s">
         <v>47</v>
       </c>
@@ -2508,31 +2515,31 @@
       <c r="A53" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="72" t="s">
+      <c r="B53" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="C53" s="72"/>
-      <c r="D53" s="74" t="s">
+      <c r="C53" s="106"/>
+      <c r="D53" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="74"/>
-      <c r="F53" s="72"/>
-      <c r="G53" s="72"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="106"/>
+      <c r="G53" s="106"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="71" t="s">
+      <c r="B54" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="C54" s="71"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="71" t="s">
+      <c r="C54" s="105"/>
+      <c r="D54" s="107"/>
+      <c r="E54" s="107"/>
+      <c r="F54" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="G54" s="71"/>
+      <c r="G54" s="105"/>
       <c r="H54" s="2" t="s">
         <v>47</v>
       </c>
@@ -2541,31 +2548,31 @@
       <c r="A55" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="72" t="s">
+      <c r="B55" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="72"/>
-      <c r="D55" s="74" t="s">
+      <c r="C55" s="106"/>
+      <c r="D55" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="E55" s="74"/>
-      <c r="F55" s="72"/>
-      <c r="G55" s="72"/>
+      <c r="E55" s="107"/>
+      <c r="F55" s="106"/>
+      <c r="G55" s="106"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="71" t="s">
+      <c r="B56" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="71"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
-      <c r="F56" s="71" t="s">
+      <c r="C56" s="105"/>
+      <c r="D56" s="107"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="G56" s="71"/>
+      <c r="G56" s="105"/>
       <c r="H56" s="2" t="s">
         <v>47</v>
       </c>
@@ -2574,14 +2581,14 @@
       <c r="A57" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B57" s="73" t="s">
+      <c r="B57" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="73"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
-      <c r="F57" s="72"/>
-      <c r="G57" s="72"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="107"/>
+      <c r="E57" s="107"/>
+      <c r="F57" s="106"/>
+      <c r="G57" s="106"/>
       <c r="H57" s="2" t="s">
         <v>100</v>
       </c>
@@ -2590,18 +2597,18 @@
       <c r="A58" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="76" t="s">
+      <c r="B58" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="C58" s="76"/>
-      <c r="D58" s="77" t="s">
+      <c r="C58" s="117"/>
+      <c r="D58" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="E58" s="77"/>
-      <c r="F58" s="76" t="s">
+      <c r="E58" s="118"/>
+      <c r="F58" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="G58" s="76"/>
+      <c r="G58" s="117"/>
       <c r="H58" s="10" t="s">
         <v>98</v>
       </c>
@@ -2610,14 +2617,14 @@
       <c r="A59" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="73" t="s">
+      <c r="B59" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="73"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="72"/>
-      <c r="G59" s="72"/>
+      <c r="C59" s="108"/>
+      <c r="D59" s="107"/>
+      <c r="E59" s="107"/>
+      <c r="F59" s="106"/>
+      <c r="G59" s="106"/>
       <c r="H59" s="2" t="s">
         <v>100</v>
       </c>
@@ -2626,14 +2633,14 @@
       <c r="A60" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="73" t="s">
+      <c r="B60" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="73"/>
-      <c r="D60" s="74"/>
-      <c r="E60" s="74"/>
-      <c r="F60" s="72"/>
-      <c r="G60" s="72"/>
+      <c r="C60" s="108"/>
+      <c r="D60" s="107"/>
+      <c r="E60" s="107"/>
+      <c r="F60" s="106"/>
+      <c r="G60" s="106"/>
       <c r="H60" s="2" t="s">
         <v>100</v>
       </c>
@@ -2642,33 +2649,33 @@
       <c r="A61" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="72" t="s">
+      <c r="B61" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="C61" s="72"/>
-      <c r="D61" s="74" t="s">
+      <c r="C61" s="106"/>
+      <c r="D61" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="74"/>
-      <c r="F61" s="72"/>
-      <c r="G61" s="72"/>
+      <c r="E61" s="107"/>
+      <c r="F61" s="106"/>
+      <c r="G61" s="106"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="76" t="s">
+      <c r="B62" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="76"/>
-      <c r="D62" s="77" t="s">
+      <c r="C62" s="117"/>
+      <c r="D62" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="77"/>
-      <c r="F62" s="76" t="s">
+      <c r="E62" s="118"/>
+      <c r="F62" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="G62" s="76"/>
+      <c r="G62" s="117"/>
       <c r="H62" s="10" t="s">
         <v>98</v>
       </c>
@@ -2677,46 +2684,46 @@
       <c r="A63" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="74" t="s">
+      <c r="B63" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="74"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="72"/>
-      <c r="G63" s="72"/>
+      <c r="C63" s="107"/>
+      <c r="D63" s="107"/>
+      <c r="E63" s="107"/>
+      <c r="F63" s="106"/>
+      <c r="G63" s="106"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="72" t="s">
+      <c r="B64" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="74" t="s">
+      <c r="C64" s="106"/>
+      <c r="D64" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="E64" s="74"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="72"/>
+      <c r="E64" s="107"/>
+      <c r="F64" s="106"/>
+      <c r="G64" s="106"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="B65" s="76" t="s">
+      <c r="B65" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="C65" s="76"/>
-      <c r="D65" s="77" t="s">
+      <c r="C65" s="117"/>
+      <c r="D65" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="E65" s="77"/>
-      <c r="F65" s="76" t="s">
+      <c r="E65" s="118"/>
+      <c r="F65" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="G65" s="76"/>
+      <c r="G65" s="117"/>
       <c r="H65" s="10" t="s">
         <v>98</v>
       </c>
@@ -2725,46 +2732,46 @@
       <c r="A66" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="74" t="s">
+      <c r="B66" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="C66" s="74"/>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="72"/>
+      <c r="C66" s="107"/>
+      <c r="D66" s="107"/>
+      <c r="E66" s="107"/>
+      <c r="F66" s="106"/>
+      <c r="G66" s="106"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="72"/>
-      <c r="D67" s="74" t="s">
+      <c r="C67" s="106"/>
+      <c r="D67" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="E67" s="74"/>
-      <c r="F67" s="72"/>
-      <c r="G67" s="72"/>
+      <c r="E67" s="107"/>
+      <c r="F67" s="106"/>
+      <c r="G67" s="106"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="76" t="s">
+      <c r="B68" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="C68" s="76"/>
-      <c r="D68" s="77" t="s">
+      <c r="C68" s="117"/>
+      <c r="D68" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="E68" s="77"/>
-      <c r="F68" s="76" t="s">
+      <c r="E68" s="118"/>
+      <c r="F68" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="G68" s="76"/>
+      <c r="G68" s="117"/>
       <c r="H68" s="10" t="s">
         <v>98</v>
       </c>
@@ -2773,16 +2780,16 @@
       <c r="A69" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="73" t="s">
+      <c r="B69" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C69" s="73"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="72"/>
-      <c r="F69" s="78" t="s">
+      <c r="C69" s="108"/>
+      <c r="D69" s="106"/>
+      <c r="E69" s="106"/>
+      <c r="F69" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="G69" s="78"/>
+      <c r="G69" s="110"/>
       <c r="H69" s="2" t="s">
         <v>102</v>
       </c>
@@ -2792,14 +2799,14 @@
       <c r="A70" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="73" t="s">
+      <c r="B70" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="73"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72"/>
-      <c r="F70" s="78"/>
-      <c r="G70" s="78"/>
+      <c r="C70" s="108"/>
+      <c r="D70" s="106"/>
+      <c r="E70" s="106"/>
+      <c r="F70" s="110"/>
+      <c r="G70" s="110"/>
       <c r="H70" s="2" t="s">
         <v>103</v>
       </c>
@@ -2808,95 +2815,95 @@
       <c r="A71" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B71" s="73" t="s">
+      <c r="B71" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="73"/>
-      <c r="D71" s="72"/>
-      <c r="E71" s="72"/>
-      <c r="F71" s="78"/>
-      <c r="G71" s="78"/>
+      <c r="C71" s="108"/>
+      <c r="D71" s="106"/>
+      <c r="E71" s="106"/>
+      <c r="F71" s="110"/>
+      <c r="G71" s="110"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="73" t="s">
+      <c r="B72" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C72" s="73"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
+      <c r="C72" s="108"/>
+      <c r="D72" s="106"/>
+      <c r="E72" s="106"/>
+      <c r="F72" s="110"/>
+      <c r="G72" s="110"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="73" t="s">
+      <c r="B73" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="73"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="78"/>
-      <c r="G73" s="78"/>
+      <c r="C73" s="108"/>
+      <c r="D73" s="106"/>
+      <c r="E73" s="106"/>
+      <c r="F73" s="110"/>
+      <c r="G73" s="110"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B74" s="73" t="s">
+      <c r="B74" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C74" s="73"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="72"/>
-      <c r="F74" s="78"/>
-      <c r="G74" s="78"/>
+      <c r="C74" s="108"/>
+      <c r="D74" s="106"/>
+      <c r="E74" s="106"/>
+      <c r="F74" s="110"/>
+      <c r="G74" s="110"/>
       <c r="H74" s="57"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B75" s="73" t="s">
+      <c r="B75" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="73"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="72"/>
-      <c r="F75" s="78"/>
-      <c r="G75" s="78"/>
+      <c r="C75" s="108"/>
+      <c r="D75" s="106"/>
+      <c r="E75" s="106"/>
+      <c r="F75" s="110"/>
+      <c r="G75" s="110"/>
       <c r="H75" s="57"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B76" s="73" t="s">
+      <c r="B76" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="73"/>
-      <c r="D76" s="72"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="78"/>
-      <c r="G76" s="78"/>
+      <c r="C76" s="108"/>
+      <c r="D76" s="106"/>
+      <c r="E76" s="106"/>
+      <c r="F76" s="110"/>
+      <c r="G76" s="110"/>
       <c r="H76" s="57"/>
     </row>
     <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B77" s="73" t="s">
+      <c r="B77" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C77" s="73"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="78"/>
-      <c r="G77" s="78"/>
+      <c r="C77" s="108"/>
+      <c r="D77" s="106"/>
+      <c r="E77" s="106"/>
+      <c r="F77" s="110"/>
+      <c r="G77" s="110"/>
       <c r="H77" s="57" t="s">
         <v>96</v>
       </c>
@@ -2905,14 +2912,14 @@
       <c r="A78" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B78" s="73" t="s">
+      <c r="B78" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C78" s="73"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="78"/>
-      <c r="G78" s="78"/>
+      <c r="C78" s="108"/>
+      <c r="D78" s="106"/>
+      <c r="E78" s="106"/>
+      <c r="F78" s="110"/>
+      <c r="G78" s="110"/>
       <c r="H78" s="57" t="s">
         <v>87</v>
       </c>
@@ -2921,14 +2928,14 @@
       <c r="A79" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B79" s="73" t="s">
+      <c r="B79" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C79" s="73"/>
-      <c r="D79" s="72"/>
-      <c r="E79" s="72"/>
-      <c r="F79" s="78"/>
-      <c r="G79" s="78"/>
+      <c r="C79" s="108"/>
+      <c r="D79" s="106"/>
+      <c r="E79" s="106"/>
+      <c r="F79" s="110"/>
+      <c r="G79" s="110"/>
       <c r="H79" s="57" t="s">
         <v>88</v>
       </c>
@@ -2937,14 +2944,14 @@
       <c r="A80" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B80" s="73" t="s">
+      <c r="B80" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="73"/>
-      <c r="D80" s="72"/>
-      <c r="E80" s="72"/>
-      <c r="F80" s="78"/>
-      <c r="G80" s="78"/>
+      <c r="C80" s="108"/>
+      <c r="D80" s="106"/>
+      <c r="E80" s="106"/>
+      <c r="F80" s="110"/>
+      <c r="G80" s="110"/>
       <c r="H80" s="57" t="s">
         <v>89</v>
       </c>
@@ -2953,150 +2960,150 @@
       <c r="A81" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B81" s="73" t="s">
+      <c r="B81" s="108" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="73"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="72"/>
-      <c r="F81" s="78"/>
-      <c r="G81" s="78"/>
+      <c r="C81" s="108"/>
+      <c r="D81" s="106"/>
+      <c r="E81" s="106"/>
+      <c r="F81" s="110"/>
+      <c r="G81" s="110"/>
       <c r="H81" s="57"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B82" s="72" t="s">
+      <c r="B82" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="C82" s="72"/>
-      <c r="D82" s="72"/>
-      <c r="E82" s="72"/>
+      <c r="C82" s="106"/>
+      <c r="D82" s="106"/>
+      <c r="E82" s="106"/>
       <c r="F82" s="52"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B83" s="74" t="s">
+      <c r="B83" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="C83" s="74"/>
-      <c r="D83" s="72"/>
-      <c r="E83" s="72"/>
+      <c r="C83" s="107"/>
+      <c r="D83" s="106"/>
+      <c r="E83" s="106"/>
       <c r="F83" s="52"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B84" s="74" t="s">
+      <c r="B84" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="C84" s="74"/>
-      <c r="D84" s="72"/>
-      <c r="E84" s="72"/>
+      <c r="C84" s="107"/>
+      <c r="D84" s="106"/>
+      <c r="E84" s="106"/>
       <c r="F84" s="52"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B85" s="72" t="s">
+      <c r="B85" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C85" s="72"/>
-      <c r="D85" s="74"/>
-      <c r="E85" s="74"/>
+      <c r="C85" s="106"/>
+      <c r="D85" s="107"/>
+      <c r="E85" s="107"/>
       <c r="F85" s="52"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B86" s="72" t="s">
+      <c r="B86" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C86" s="72"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
+      <c r="C86" s="106"/>
+      <c r="D86" s="107"/>
+      <c r="E86" s="107"/>
       <c r="F86" s="52"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B87" s="72" t="s">
+      <c r="B87" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C87" s="72"/>
-      <c r="D87" s="74"/>
-      <c r="E87" s="74"/>
+      <c r="C87" s="106"/>
+      <c r="D87" s="107"/>
+      <c r="E87" s="107"/>
       <c r="F87" s="52"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B88" s="72" t="s">
+      <c r="B88" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C88" s="72"/>
-      <c r="D88" s="74"/>
-      <c r="E88" s="74"/>
+      <c r="C88" s="106"/>
+      <c r="D88" s="107"/>
+      <c r="E88" s="107"/>
       <c r="F88" s="52"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B89" s="72" t="s">
+      <c r="B89" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C89" s="72"/>
-      <c r="D89" s="74"/>
-      <c r="E89" s="74"/>
+      <c r="C89" s="106"/>
+      <c r="D89" s="107"/>
+      <c r="E89" s="107"/>
       <c r="F89" s="52"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B90" s="72" t="s">
+      <c r="B90" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C90" s="72"/>
-      <c r="D90" s="74"/>
-      <c r="E90" s="74"/>
+      <c r="C90" s="106"/>
+      <c r="D90" s="107"/>
+      <c r="E90" s="107"/>
       <c r="F90" s="52"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B91" s="72" t="s">
+      <c r="B91" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C91" s="72"/>
-      <c r="D91" s="74"/>
-      <c r="E91" s="74"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="107"/>
+      <c r="E91" s="107"/>
       <c r="F91" s="52"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B92" s="73" t="s">
+      <c r="B92" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="C92" s="73"/>
-      <c r="D92" s="73"/>
-      <c r="E92" s="73"/>
-      <c r="F92" s="73" t="s">
+      <c r="C92" s="108"/>
+      <c r="D92" s="108"/>
+      <c r="E92" s="108"/>
+      <c r="F92" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="G92" s="73"/>
+      <c r="G92" s="108"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="55"/>
@@ -3108,134 +3115,134 @@
       <c r="A95" s="53"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B96" s="75" t="s">
+      <c r="B96" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="75"/>
-      <c r="D96" s="75" t="s">
+      <c r="C96" s="116"/>
+      <c r="D96" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="E96" s="75"/>
-      <c r="F96" s="72" t="s">
+      <c r="E96" s="116"/>
+      <c r="F96" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="G96" s="72"/>
+      <c r="G96" s="106"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B97" s="72" t="s">
+      <c r="B97" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C97" s="72"/>
-      <c r="D97" s="72"/>
-      <c r="E97" s="72"/>
-      <c r="F97" s="72"/>
-      <c r="G97" s="72"/>
+      <c r="C97" s="106"/>
+      <c r="D97" s="106"/>
+      <c r="E97" s="106"/>
+      <c r="F97" s="106"/>
+      <c r="G97" s="106"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B98" s="79" t="s">
+      <c r="B98" s="113" t="s">
         <v>104</v>
       </c>
-      <c r="C98" s="79"/>
-      <c r="D98" s="80" t="s">
+      <c r="C98" s="113"/>
+      <c r="D98" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="E98" s="80"/>
-      <c r="F98" s="72"/>
-      <c r="G98" s="72"/>
+      <c r="E98" s="111"/>
+      <c r="F98" s="106"/>
+      <c r="G98" s="106"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="B99" s="81" t="s">
+      <c r="B99" s="114" t="s">
         <v>99</v>
       </c>
-      <c r="C99" s="81"/>
-      <c r="D99" s="82"/>
-      <c r="E99" s="82"/>
-      <c r="F99" s="81" t="s">
+      <c r="C99" s="114"/>
+      <c r="D99" s="115"/>
+      <c r="E99" s="115"/>
+      <c r="F99" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="G99" s="81"/>
+      <c r="G99" s="114"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="79" t="s">
+      <c r="B100" s="113" t="s">
         <v>104</v>
       </c>
-      <c r="C100" s="79"/>
-      <c r="D100" s="80" t="s">
+      <c r="C100" s="113"/>
+      <c r="D100" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="E100" s="80"/>
-      <c r="F100" s="72"/>
-      <c r="G100" s="72"/>
+      <c r="E100" s="111"/>
+      <c r="F100" s="106"/>
+      <c r="G100" s="106"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B101" s="81" t="s">
+      <c r="B101" s="114" t="s">
         <v>99</v>
       </c>
-      <c r="C101" s="81"/>
-      <c r="D101" s="82"/>
-      <c r="E101" s="82"/>
-      <c r="F101" s="81" t="s">
+      <c r="C101" s="114"/>
+      <c r="D101" s="115"/>
+      <c r="E101" s="115"/>
+      <c r="F101" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="G101" s="81"/>
+      <c r="G101" s="114"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="79" t="s">
+      <c r="B102" s="113" t="s">
         <v>104</v>
       </c>
-      <c r="C102" s="79"/>
-      <c r="D102" s="80" t="s">
+      <c r="C102" s="113"/>
+      <c r="D102" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="E102" s="80"/>
-      <c r="F102" s="72"/>
-      <c r="G102" s="72"/>
+      <c r="E102" s="111"/>
+      <c r="F102" s="106"/>
+      <c r="G102" s="106"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="B103" s="81" t="s">
+      <c r="B103" s="114" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="81"/>
-      <c r="D103" s="82"/>
-      <c r="E103" s="82"/>
-      <c r="F103" s="81" t="s">
+      <c r="C103" s="114"/>
+      <c r="D103" s="115"/>
+      <c r="E103" s="115"/>
+      <c r="F103" s="114" t="s">
         <v>92</v>
       </c>
-      <c r="G103" s="81"/>
+      <c r="G103" s="114"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B104" s="83"/>
-      <c r="C104" s="83"/>
-      <c r="D104" s="83" t="s">
+      <c r="B104" s="109"/>
+      <c r="C104" s="109"/>
+      <c r="D104" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E104" s="83"/>
-      <c r="F104" s="84"/>
-      <c r="G104" s="84"/>
+      <c r="E104" s="109"/>
+      <c r="F104" s="112"/>
+      <c r="G104" s="112"/>
       <c r="H104" s="68" t="s">
         <v>100</v>
       </c>
@@ -3244,14 +3251,14 @@
       <c r="A105" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B105" s="83"/>
-      <c r="C105" s="83"/>
-      <c r="D105" s="83" t="s">
+      <c r="B105" s="109"/>
+      <c r="C105" s="109"/>
+      <c r="D105" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E105" s="83"/>
-      <c r="F105" s="84"/>
-      <c r="G105" s="84"/>
+      <c r="E105" s="109"/>
+      <c r="F105" s="112"/>
+      <c r="G105" s="112"/>
       <c r="H105" s="68" t="s">
         <v>100</v>
       </c>
@@ -3260,14 +3267,14 @@
       <c r="A106" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B106" s="83"/>
-      <c r="C106" s="83"/>
-      <c r="D106" s="83" t="s">
+      <c r="B106" s="109"/>
+      <c r="C106" s="109"/>
+      <c r="D106" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E106" s="83"/>
-      <c r="F106" s="84"/>
-      <c r="G106" s="84"/>
+      <c r="E106" s="109"/>
+      <c r="F106" s="112"/>
+      <c r="G106" s="112"/>
       <c r="H106" s="68" t="s">
         <v>100</v>
       </c>
@@ -3276,87 +3283,87 @@
       <c r="A107" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B107" s="74" t="s">
+      <c r="B107" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="C107" s="74"/>
-      <c r="D107" s="74" t="s">
+      <c r="C107" s="107"/>
+      <c r="D107" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="E107" s="74"/>
-      <c r="F107" s="72"/>
-      <c r="G107" s="72"/>
+      <c r="E107" s="107"/>
+      <c r="F107" s="106"/>
+      <c r="G107" s="106"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="80"/>
-      <c r="C108" s="80"/>
-      <c r="D108" s="80" t="s">
+      <c r="B108" s="111"/>
+      <c r="C108" s="111"/>
+      <c r="D108" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="E108" s="80"/>
-      <c r="F108" s="72"/>
-      <c r="G108" s="72"/>
+      <c r="E108" s="111"/>
+      <c r="F108" s="106"/>
+      <c r="G108" s="106"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="74" t="s">
+      <c r="B109" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="C109" s="74"/>
-      <c r="D109" s="74" t="s">
+      <c r="C109" s="107"/>
+      <c r="D109" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="E109" s="74"/>
-      <c r="F109" s="72"/>
-      <c r="G109" s="72"/>
+      <c r="E109" s="107"/>
+      <c r="F109" s="106"/>
+      <c r="G109" s="106"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="80"/>
-      <c r="C110" s="80"/>
-      <c r="D110" s="80" t="s">
+      <c r="B110" s="111"/>
+      <c r="C110" s="111"/>
+      <c r="D110" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="E110" s="80"/>
-      <c r="F110" s="72"/>
-      <c r="G110" s="72"/>
+      <c r="E110" s="111"/>
+      <c r="F110" s="106"/>
+      <c r="G110" s="106"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="74" t="s">
+      <c r="B111" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="C111" s="74"/>
-      <c r="D111" s="74" t="s">
+      <c r="C111" s="107"/>
+      <c r="D111" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="E111" s="74"/>
-      <c r="F111" s="72"/>
-      <c r="G111" s="72"/>
+      <c r="E111" s="107"/>
+      <c r="F111" s="106"/>
+      <c r="G111" s="106"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="83"/>
-      <c r="C112" s="83"/>
-      <c r="D112" s="83" t="s">
+      <c r="B112" s="109"/>
+      <c r="C112" s="109"/>
+      <c r="D112" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E112" s="83"/>
-      <c r="F112" s="78" t="s">
+      <c r="E112" s="109"/>
+      <c r="F112" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="G112" s="78"/>
+      <c r="G112" s="110"/>
       <c r="H112" s="68" t="s">
         <v>102</v>
       </c>
@@ -3365,14 +3372,14 @@
       <c r="A113" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B113" s="83"/>
-      <c r="C113" s="83"/>
-      <c r="D113" s="83" t="s">
+      <c r="B113" s="109"/>
+      <c r="C113" s="109"/>
+      <c r="D113" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E113" s="83"/>
-      <c r="F113" s="78"/>
-      <c r="G113" s="78"/>
+      <c r="E113" s="109"/>
+      <c r="F113" s="110"/>
+      <c r="G113" s="110"/>
       <c r="H113" s="68" t="s">
         <v>103</v>
       </c>
@@ -3381,95 +3388,95 @@
       <c r="A114" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B114" s="85" t="s">
+      <c r="B114" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="C114" s="85"/>
-      <c r="D114" s="85"/>
-      <c r="E114" s="85"/>
-      <c r="F114" s="78"/>
-      <c r="G114" s="78"/>
+      <c r="C114" s="104"/>
+      <c r="D114" s="104"/>
+      <c r="E114" s="104"/>
+      <c r="F114" s="110"/>
+      <c r="G114" s="110"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B115" s="83"/>
-      <c r="C115" s="83"/>
-      <c r="D115" s="83" t="s">
+      <c r="B115" s="109"/>
+      <c r="C115" s="109"/>
+      <c r="D115" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E115" s="83"/>
-      <c r="F115" s="78"/>
-      <c r="G115" s="78"/>
+      <c r="E115" s="109"/>
+      <c r="F115" s="110"/>
+      <c r="G115" s="110"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B116" s="83"/>
-      <c r="C116" s="83"/>
-      <c r="D116" s="83" t="s">
+      <c r="B116" s="109"/>
+      <c r="C116" s="109"/>
+      <c r="D116" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E116" s="83"/>
-      <c r="F116" s="78"/>
-      <c r="G116" s="78"/>
+      <c r="E116" s="109"/>
+      <c r="F116" s="110"/>
+      <c r="G116" s="110"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B117" s="83"/>
-      <c r="C117" s="83"/>
-      <c r="D117" s="83" t="s">
+      <c r="B117" s="109"/>
+      <c r="C117" s="109"/>
+      <c r="D117" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E117" s="83"/>
-      <c r="F117" s="78"/>
-      <c r="G117" s="78"/>
+      <c r="E117" s="109"/>
+      <c r="F117" s="110"/>
+      <c r="G117" s="110"/>
       <c r="H117" s="57"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B118" s="83"/>
-      <c r="C118" s="83"/>
-      <c r="D118" s="83" t="s">
+      <c r="B118" s="109"/>
+      <c r="C118" s="109"/>
+      <c r="D118" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E118" s="83"/>
-      <c r="F118" s="78"/>
-      <c r="G118" s="78"/>
+      <c r="E118" s="109"/>
+      <c r="F118" s="110"/>
+      <c r="G118" s="110"/>
       <c r="H118" s="57"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B119" s="83"/>
-      <c r="C119" s="83"/>
-      <c r="D119" s="83" t="s">
+      <c r="B119" s="109"/>
+      <c r="C119" s="109"/>
+      <c r="D119" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E119" s="83"/>
-      <c r="F119" s="78"/>
-      <c r="G119" s="78"/>
+      <c r="E119" s="109"/>
+      <c r="F119" s="110"/>
+      <c r="G119" s="110"/>
       <c r="H119" s="57"/>
     </row>
     <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B120" s="83"/>
-      <c r="C120" s="83"/>
-      <c r="D120" s="83" t="s">
+      <c r="B120" s="109"/>
+      <c r="C120" s="109"/>
+      <c r="D120" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E120" s="83"/>
-      <c r="F120" s="78"/>
-      <c r="G120" s="78"/>
+      <c r="E120" s="109"/>
+      <c r="F120" s="110"/>
+      <c r="G120" s="110"/>
       <c r="H120" s="57" t="s">
         <v>96</v>
       </c>
@@ -3478,14 +3485,14 @@
       <c r="A121" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B121" s="85" t="s">
+      <c r="B121" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="C121" s="85"/>
-      <c r="D121" s="85"/>
-      <c r="E121" s="85"/>
-      <c r="F121" s="78"/>
-      <c r="G121" s="78"/>
+      <c r="C121" s="104"/>
+      <c r="D121" s="104"/>
+      <c r="E121" s="104"/>
+      <c r="F121" s="110"/>
+      <c r="G121" s="110"/>
       <c r="H121" s="57" t="s">
         <v>87</v>
       </c>
@@ -3494,14 +3501,14 @@
       <c r="A122" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B122" s="83"/>
-      <c r="C122" s="83"/>
-      <c r="D122" s="83" t="s">
+      <c r="B122" s="109"/>
+      <c r="C122" s="109"/>
+      <c r="D122" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E122" s="83"/>
-      <c r="F122" s="78"/>
-      <c r="G122" s="78"/>
+      <c r="E122" s="109"/>
+      <c r="F122" s="110"/>
+      <c r="G122" s="110"/>
       <c r="H122" s="57" t="s">
         <v>88</v>
       </c>
@@ -3510,14 +3517,14 @@
       <c r="A123" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B123" s="83"/>
-      <c r="C123" s="83"/>
-      <c r="D123" s="83" t="s">
+      <c r="B123" s="109"/>
+      <c r="C123" s="109"/>
+      <c r="D123" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E123" s="83"/>
-      <c r="F123" s="78"/>
-      <c r="G123" s="78"/>
+      <c r="E123" s="109"/>
+      <c r="F123" s="110"/>
+      <c r="G123" s="110"/>
       <c r="H123" s="57" t="s">
         <v>89</v>
       </c>
@@ -3526,26 +3533,26 @@
       <c r="A124" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B124" s="83"/>
-      <c r="C124" s="83"/>
-      <c r="D124" s="83" t="s">
+      <c r="B124" s="109"/>
+      <c r="C124" s="109"/>
+      <c r="D124" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="E124" s="83"/>
-      <c r="F124" s="78"/>
-      <c r="G124" s="78"/>
+      <c r="E124" s="109"/>
+      <c r="F124" s="110"/>
+      <c r="G124" s="110"/>
       <c r="H124" s="57"/>
     </row>
     <row r="125" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B125" s="71" t="s">
+      <c r="B125" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="C125" s="71"/>
-      <c r="D125" s="71"/>
-      <c r="E125" s="71"/>
+      <c r="C125" s="105"/>
+      <c r="D125" s="105"/>
+      <c r="E125" s="105"/>
       <c r="F125" s="51"/>
       <c r="G125" s="60"/>
       <c r="H125" s="69" t="s">
@@ -3556,12 +3563,12 @@
       <c r="A126" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B126" s="85" t="s">
+      <c r="B126" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="C126" s="85"/>
-      <c r="D126" s="71"/>
-      <c r="E126" s="71"/>
+      <c r="C126" s="104"/>
+      <c r="D126" s="105"/>
+      <c r="E126" s="105"/>
       <c r="F126" s="51"/>
       <c r="G126" s="60"/>
       <c r="H126" s="69" t="s">
@@ -3572,12 +3579,12 @@
       <c r="A127" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B127" s="85" t="s">
+      <c r="B127" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="C127" s="85"/>
-      <c r="D127" s="71"/>
-      <c r="E127" s="71"/>
+      <c r="C127" s="104"/>
+      <c r="D127" s="105"/>
+      <c r="E127" s="105"/>
       <c r="F127" s="51"/>
       <c r="G127" s="60"/>
       <c r="H127" s="69" t="s">
@@ -3588,12 +3595,12 @@
       <c r="A128" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B128" s="72" t="s">
+      <c r="B128" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C128" s="72"/>
-      <c r="D128" s="74"/>
-      <c r="E128" s="74"/>
+      <c r="C128" s="106"/>
+      <c r="D128" s="107"/>
+      <c r="E128" s="107"/>
       <c r="F128" s="52"/>
       <c r="G128" s="59"/>
     </row>
@@ -3601,12 +3608,12 @@
       <c r="A129" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B129" s="72" t="s">
+      <c r="B129" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C129" s="72"/>
-      <c r="D129" s="74"/>
-      <c r="E129" s="74"/>
+      <c r="C129" s="106"/>
+      <c r="D129" s="107"/>
+      <c r="E129" s="107"/>
       <c r="F129" s="52"/>
       <c r="G129" s="59"/>
     </row>
@@ -3614,12 +3621,12 @@
       <c r="A130" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B130" s="72" t="s">
+      <c r="B130" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C130" s="72"/>
-      <c r="D130" s="74"/>
-      <c r="E130" s="74"/>
+      <c r="C130" s="106"/>
+      <c r="D130" s="107"/>
+      <c r="E130" s="107"/>
       <c r="F130" s="52"/>
       <c r="G130" s="59"/>
     </row>
@@ -3627,12 +3634,12 @@
       <c r="A131" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B131" s="72" t="s">
+      <c r="B131" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C131" s="72"/>
-      <c r="D131" s="74"/>
-      <c r="E131" s="74"/>
+      <c r="C131" s="106"/>
+      <c r="D131" s="107"/>
+      <c r="E131" s="107"/>
       <c r="F131" s="52"/>
       <c r="G131" s="59"/>
     </row>
@@ -3640,12 +3647,12 @@
       <c r="A132" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B132" s="72" t="s">
+      <c r="B132" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C132" s="72"/>
-      <c r="D132" s="74"/>
-      <c r="E132" s="74"/>
+      <c r="C132" s="106"/>
+      <c r="D132" s="107"/>
+      <c r="E132" s="107"/>
       <c r="F132" s="52"/>
       <c r="G132" s="59"/>
     </row>
@@ -3653,12 +3660,12 @@
       <c r="A133" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B133" s="72" t="s">
+      <c r="B133" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C133" s="72"/>
-      <c r="D133" s="74"/>
-      <c r="E133" s="74"/>
+      <c r="C133" s="106"/>
+      <c r="D133" s="107"/>
+      <c r="E133" s="107"/>
       <c r="F133" s="52"/>
       <c r="G133" s="59"/>
     </row>
@@ -3666,12 +3673,12 @@
       <c r="A134" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B134" s="72" t="s">
+      <c r="B134" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C134" s="72"/>
-      <c r="D134" s="74"/>
-      <c r="E134" s="74"/>
+      <c r="C134" s="106"/>
+      <c r="D134" s="107"/>
+      <c r="E134" s="107"/>
       <c r="F134" s="52"/>
       <c r="G134" s="59"/>
     </row>
@@ -3679,48 +3686,174 @@
       <c r="A135" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B135" s="73" t="s">
+      <c r="B135" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="C135" s="73"/>
-      <c r="D135" s="73"/>
-      <c r="E135" s="73"/>
-      <c r="F135" s="73" t="s">
+      <c r="C135" s="108"/>
+      <c r="D135" s="108"/>
+      <c r="E135" s="108"/>
+      <c r="F135" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="G135" s="73"/>
+      <c r="G135" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="208">
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="F135:G135"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F92:G92"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F69:G81"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="F97:G97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="F98:G98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="F106:G106"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="F104:G104"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="F109:G109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="F107:G107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:G108"/>
     <mergeCell ref="B111:C111"/>
     <mergeCell ref="D111:E111"/>
     <mergeCell ref="F111:G111"/>
@@ -3745,161 +3878,35 @@
     <mergeCell ref="D120:E120"/>
     <mergeCell ref="B121:C121"/>
     <mergeCell ref="D121:E121"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="F109:G109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="F110:G110"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="F107:G107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="F106:G106"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="F104:G104"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="F97:G97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="F98:G98"/>
-    <mergeCell ref="F92:G92"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F69:G81"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="F135:G135"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:E134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3909,8 +3916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18896507-0B9C-B34F-BC05-0C78932B60CE}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3923,887 +3930,1796 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="64" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86"/>
-      <c r="B1" s="86" t="s">
+      <c r="A1" s="73"/>
+      <c r="B1" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="73" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="88" t="s">
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="89">
-        <v>0</v>
-      </c>
-      <c r="D2" s="90">
+      <c r="C2" s="76">
+        <v>0</v>
+      </c>
+      <c r="D2" s="77">
         <f>C2/858</f>
         <v>0</v>
       </c>
-      <c r="E2" s="89">
+      <c r="E2" s="76">
         <v>13</v>
       </c>
-      <c r="F2" s="89">
+      <c r="F2" s="76">
         <v>84</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="76" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="93">
+      <c r="A3" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="80">
         <v>26</v>
       </c>
-      <c r="D3" s="94">
+      <c r="D3" s="81">
         <f t="shared" ref="D3:D37" si="0">C3/858</f>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="E3" s="93">
-        <v>1</v>
-      </c>
-      <c r="F3" s="93">
+      <c r="E3" s="80">
+        <v>1</v>
+      </c>
+      <c r="F3" s="80">
         <v>28</v>
       </c>
-      <c r="G3" s="93" t="s">
+      <c r="G3" s="80" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="89">
+      <c r="B4" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="76">
         <v>7</v>
       </c>
-      <c r="D4" s="95">
+      <c r="D4" s="82">
         <f t="shared" si="0"/>
         <v>8.1585081585081581E-3</v>
       </c>
-      <c r="E4" s="89">
+      <c r="E4" s="76">
         <v>10</v>
       </c>
-      <c r="F4" s="89">
+      <c r="F4" s="76">
         <v>32</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="76" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="93">
+      <c r="B5" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="80">
         <v>56</v>
       </c>
-      <c r="D5" s="94">
+      <c r="D5" s="81">
         <f t="shared" si="0"/>
         <v>6.5268065268065265E-2</v>
       </c>
-      <c r="E5" s="93">
-        <v>0</v>
-      </c>
-      <c r="F5" s="93">
+      <c r="E5" s="80">
+        <v>0</v>
+      </c>
+      <c r="F5" s="80">
         <v>11</v>
       </c>
-      <c r="G5" s="93" t="s">
+      <c r="G5" s="80" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="97" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="98">
+      <c r="B6" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="85">
         <v>13</v>
       </c>
-      <c r="D6" s="99">
+      <c r="D6" s="86">
         <f t="shared" si="0"/>
         <v>1.5151515151515152E-2</v>
       </c>
-      <c r="E6" s="98">
-        <v>0</v>
-      </c>
-      <c r="F6" s="98">
-        <v>1</v>
-      </c>
-      <c r="G6" s="98" t="s">
+      <c r="E6" s="85">
+        <v>0</v>
+      </c>
+      <c r="F6" s="85">
+        <v>1</v>
+      </c>
+      <c r="G6" s="85" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="89">
+      <c r="B7" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="76">
         <v>13</v>
       </c>
-      <c r="D7" s="95">
+      <c r="D7" s="82">
         <f t="shared" si="0"/>
         <v>1.5151515151515152E-2</v>
       </c>
-      <c r="E7" s="89">
-        <v>0</v>
-      </c>
-      <c r="F7" s="89">
+      <c r="E7" s="76">
+        <v>0</v>
+      </c>
+      <c r="F7" s="76">
         <v>37</v>
       </c>
-      <c r="G7" s="89" t="s">
+      <c r="G7" s="76" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="89">
+      <c r="B8" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="76">
         <v>13</v>
       </c>
-      <c r="D8" s="95">
+      <c r="D8" s="82">
         <f t="shared" si="0"/>
         <v>1.5151515151515152E-2</v>
       </c>
-      <c r="E8" s="89">
-        <v>0</v>
-      </c>
-      <c r="F8" s="89">
+      <c r="E8" s="76">
+        <v>0</v>
+      </c>
+      <c r="F8" s="76">
         <v>37</v>
       </c>
-      <c r="G8" s="89" t="s">
+      <c r="G8" s="76" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="39" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="101" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="102">
+      <c r="B9" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="89">
         <v>108</v>
       </c>
-      <c r="D9" s="103">
+      <c r="D9" s="90">
         <f t="shared" si="0"/>
         <v>0.12587412587412589</v>
       </c>
-      <c r="E9" s="102">
-        <v>0</v>
-      </c>
-      <c r="F9" s="102">
-        <v>1</v>
-      </c>
-      <c r="G9" s="102" t="s">
+      <c r="E9" s="89">
+        <v>0</v>
+      </c>
+      <c r="F9" s="89">
+        <v>1</v>
+      </c>
+      <c r="G9" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="105" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="106">
+      <c r="B10" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="93">
         <v>108</v>
       </c>
-      <c r="D10" s="107">
+      <c r="D10" s="94">
         <f t="shared" si="0"/>
         <v>0.12587412587412589</v>
       </c>
-      <c r="E10" s="106">
-        <v>0</v>
-      </c>
-      <c r="F10" s="106">
+      <c r="E10" s="93">
+        <v>0</v>
+      </c>
+      <c r="F10" s="93">
         <v>30</v>
       </c>
-      <c r="G10" s="106" t="s">
+      <c r="G10" s="93" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="40" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="97" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="98">
+      <c r="B11" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="85">
         <v>117</v>
       </c>
-      <c r="D11" s="99">
+      <c r="D11" s="86">
         <f t="shared" si="0"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="E11" s="98">
-        <v>0</v>
-      </c>
-      <c r="F11" s="98">
-        <v>1</v>
-      </c>
-      <c r="G11" s="98" t="s">
+      <c r="E11" s="85">
+        <v>0</v>
+      </c>
+      <c r="F11" s="85">
+        <v>1</v>
+      </c>
+      <c r="G11" s="85" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="88" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="89">
+      <c r="B12" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="76">
         <v>117</v>
       </c>
-      <c r="D12" s="95">
+      <c r="D12" s="82">
         <f t="shared" si="0"/>
         <v>0.13636363636363635</v>
       </c>
-      <c r="E12" s="89">
-        <v>0</v>
-      </c>
-      <c r="F12" s="89">
+      <c r="E12" s="76">
+        <v>0</v>
+      </c>
+      <c r="F12" s="76">
         <v>19</v>
       </c>
-      <c r="G12" s="89" t="s">
+      <c r="G12" s="76" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="40" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="109" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="110">
+      <c r="B13" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="97">
         <v>105</v>
       </c>
-      <c r="D13" s="111">
+      <c r="D13" s="98">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E13" s="110">
-        <v>0</v>
-      </c>
-      <c r="F13" s="110">
-        <v>1</v>
-      </c>
-      <c r="G13" s="110" t="s">
+      <c r="E13" s="97">
+        <v>0</v>
+      </c>
+      <c r="F13" s="97">
+        <v>1</v>
+      </c>
+      <c r="G13" s="97" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="108" t="s">
+      <c r="A14" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="109" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="110">
+      <c r="B14" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="97">
         <v>105</v>
       </c>
-      <c r="D14" s="111">
+      <c r="D14" s="98">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E14" s="110">
-        <v>0</v>
-      </c>
-      <c r="F14" s="110">
+      <c r="E14" s="97">
+        <v>0</v>
+      </c>
+      <c r="F14" s="97">
         <v>4</v>
       </c>
-      <c r="G14" s="110" t="s">
+      <c r="G14" s="97" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="91" t="s">
+      <c r="A15" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="93">
+      <c r="B15" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="80">
         <v>105</v>
       </c>
-      <c r="D15" s="94">
+      <c r="D15" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E15" s="93">
-        <v>0</v>
-      </c>
-      <c r="F15" s="93">
-        <v>1</v>
-      </c>
-      <c r="G15" s="102" t="s">
+      <c r="E15" s="80">
+        <v>0</v>
+      </c>
+      <c r="F15" s="80">
+        <v>1</v>
+      </c>
+      <c r="G15" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="93">
+      <c r="B16" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="80">
         <v>105</v>
       </c>
-      <c r="D16" s="94">
+      <c r="D16" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E16" s="93">
-        <v>0</v>
-      </c>
-      <c r="F16" s="93">
-        <v>1</v>
-      </c>
-      <c r="G16" s="102" t="s">
+      <c r="E16" s="80">
+        <v>0</v>
+      </c>
+      <c r="F16" s="80">
+        <v>1</v>
+      </c>
+      <c r="G16" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="91" t="s">
+      <c r="A17" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="93">
+      <c r="B17" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="80">
         <v>105</v>
       </c>
-      <c r="D17" s="94">
+      <c r="D17" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E17" s="93">
-        <v>0</v>
-      </c>
-      <c r="F17" s="93">
-        <v>1</v>
-      </c>
-      <c r="G17" s="102" t="s">
+      <c r="E17" s="80">
+        <v>0</v>
+      </c>
+      <c r="F17" s="80">
+        <v>1</v>
+      </c>
+      <c r="G17" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="91" t="s">
+      <c r="A18" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="93">
+      <c r="B18" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="80">
         <v>105</v>
       </c>
-      <c r="D18" s="94">
+      <c r="D18" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E18" s="93">
-        <v>0</v>
-      </c>
-      <c r="F18" s="93">
-        <v>1</v>
-      </c>
-      <c r="G18" s="102" t="s">
+      <c r="E18" s="80">
+        <v>0</v>
+      </c>
+      <c r="F18" s="80">
+        <v>1</v>
+      </c>
+      <c r="G18" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="91" t="s">
+      <c r="A19" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="93">
+      <c r="B19" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="80">
         <v>105</v>
       </c>
-      <c r="D19" s="94">
+      <c r="D19" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E19" s="93">
-        <v>0</v>
-      </c>
-      <c r="F19" s="93">
-        <v>1</v>
-      </c>
-      <c r="G19" s="102" t="s">
+      <c r="E19" s="80">
+        <v>0</v>
+      </c>
+      <c r="F19" s="80">
+        <v>1</v>
+      </c>
+      <c r="G19" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="91" t="s">
+      <c r="A20" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="93">
+      <c r="B20" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="80">
         <v>105</v>
       </c>
-      <c r="D20" s="94">
+      <c r="D20" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E20" s="93">
-        <v>0</v>
-      </c>
-      <c r="F20" s="93">
-        <v>1</v>
-      </c>
-      <c r="G20" s="102" t="s">
+      <c r="E20" s="80">
+        <v>0</v>
+      </c>
+      <c r="F20" s="80">
+        <v>1</v>
+      </c>
+      <c r="G20" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="91" t="s">
+      <c r="A21" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="93">
+      <c r="B21" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="80">
         <v>105</v>
       </c>
-      <c r="D21" s="94">
+      <c r="D21" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E21" s="93">
-        <v>0</v>
-      </c>
-      <c r="F21" s="93">
-        <v>1</v>
-      </c>
-      <c r="G21" s="102" t="s">
+      <c r="E21" s="80">
+        <v>0</v>
+      </c>
+      <c r="F21" s="80">
+        <v>1</v>
+      </c>
+      <c r="G21" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="91" t="s">
+      <c r="A22" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="93">
+      <c r="B22" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="80">
         <v>105</v>
       </c>
-      <c r="D22" s="94">
+      <c r="D22" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E22" s="93">
-        <v>0</v>
-      </c>
-      <c r="F22" s="93">
-        <v>1</v>
-      </c>
-      <c r="G22" s="102" t="s">
+      <c r="E22" s="80">
+        <v>0</v>
+      </c>
+      <c r="F22" s="80">
+        <v>1</v>
+      </c>
+      <c r="G22" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="91" t="s">
+      <c r="A23" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="93">
+      <c r="B23" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="80">
         <v>105</v>
       </c>
-      <c r="D23" s="94">
+      <c r="D23" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E23" s="93">
-        <v>0</v>
-      </c>
-      <c r="F23" s="93">
-        <v>1</v>
-      </c>
-      <c r="G23" s="102" t="s">
+      <c r="E23" s="80">
+        <v>0</v>
+      </c>
+      <c r="F23" s="80">
+        <v>1</v>
+      </c>
+      <c r="G23" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="91" t="s">
+      <c r="A24" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="93">
+      <c r="B24" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="80">
         <v>105</v>
       </c>
-      <c r="D24" s="94">
+      <c r="D24" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E24" s="93">
-        <v>0</v>
-      </c>
-      <c r="F24" s="93">
-        <v>1</v>
-      </c>
-      <c r="G24" s="102" t="s">
+      <c r="E24" s="80">
+        <v>0</v>
+      </c>
+      <c r="F24" s="80">
+        <v>1</v>
+      </c>
+      <c r="G24" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="91" t="s">
+      <c r="A25" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="93">
+      <c r="B25" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="80">
         <v>105</v>
       </c>
-      <c r="D25" s="94">
+      <c r="D25" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E25" s="93">
-        <v>0</v>
-      </c>
-      <c r="F25" s="93">
-        <v>1</v>
-      </c>
-      <c r="G25" s="102" t="s">
+      <c r="E25" s="80">
+        <v>0</v>
+      </c>
+      <c r="F25" s="80">
+        <v>1</v>
+      </c>
+      <c r="G25" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="93">
+      <c r="B26" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="80">
         <v>105</v>
       </c>
-      <c r="D26" s="94">
+      <c r="D26" s="81">
         <f t="shared" si="0"/>
         <v>0.12237762237762238</v>
       </c>
-      <c r="E26" s="93">
-        <v>0</v>
-      </c>
-      <c r="F26" s="93">
-        <v>1</v>
-      </c>
-      <c r="G26" s="102" t="s">
+      <c r="E26" s="80">
+        <v>0</v>
+      </c>
+      <c r="F26" s="80">
+        <v>1</v>
+      </c>
+      <c r="G26" s="89" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="89">
-        <v>0</v>
-      </c>
-      <c r="D27" s="95">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="89">
-        <v>0</v>
-      </c>
-      <c r="F27" s="89">
+      <c r="C27" s="76">
+        <v>0</v>
+      </c>
+      <c r="D27" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="76">
+        <v>0</v>
+      </c>
+      <c r="F27" s="76">
         <v>3</v>
       </c>
-      <c r="G27" s="89" t="s">
+      <c r="G27" s="76" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="91" t="s">
+      <c r="A28" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="93">
+      <c r="B28" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="80">
         <v>787</v>
       </c>
-      <c r="D28" s="112">
+      <c r="D28" s="99">
         <f t="shared" si="0"/>
         <v>0.91724941724941722</v>
       </c>
-      <c r="E28" s="93">
-        <v>1</v>
-      </c>
-      <c r="F28" s="93">
+      <c r="E28" s="80">
+        <v>1</v>
+      </c>
+      <c r="F28" s="80">
         <v>22</v>
       </c>
-      <c r="G28" s="93" t="s">
+      <c r="G28" s="80" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="91" t="s">
+      <c r="A29" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="92" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="93">
+      <c r="B29" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="80">
         <v>787</v>
       </c>
-      <c r="D29" s="112">
+      <c r="D29" s="99">
         <f t="shared" si="0"/>
         <v>0.91724941724941722</v>
       </c>
-      <c r="E29" s="93">
-        <v>1</v>
-      </c>
-      <c r="F29" s="93">
+      <c r="E29" s="80">
+        <v>1</v>
+      </c>
+      <c r="F29" s="80">
         <v>22</v>
       </c>
-      <c r="G29" s="93" t="s">
+      <c r="G29" s="80" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="88" t="s">
+      <c r="B30" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="89">
-        <v>0</v>
-      </c>
-      <c r="D30" s="95">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="89">
-        <v>0</v>
-      </c>
-      <c r="F30" s="89">
-        <v>1</v>
-      </c>
-      <c r="G30" s="89" t="s">
+      <c r="C30" s="76">
+        <v>0</v>
+      </c>
+      <c r="D30" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="76">
+        <v>0</v>
+      </c>
+      <c r="F30" s="76">
+        <v>1</v>
+      </c>
+      <c r="G30" s="76" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="91" t="s">
+      <c r="A31" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="93">
-        <v>0</v>
-      </c>
-      <c r="D31" s="94">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="93">
-        <v>0</v>
-      </c>
-      <c r="F31" s="93">
-        <v>1</v>
-      </c>
-      <c r="G31" s="93" t="s">
+      <c r="C31" s="80">
+        <v>0</v>
+      </c>
+      <c r="D31" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="80">
+        <v>0</v>
+      </c>
+      <c r="F31" s="80">
+        <v>1</v>
+      </c>
+      <c r="G31" s="80" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="88" t="s">
+      <c r="B32" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="89">
-        <v>0</v>
-      </c>
-      <c r="D32" s="95">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="89">
-        <v>0</v>
-      </c>
-      <c r="F32" s="89">
-        <v>1</v>
-      </c>
-      <c r="G32" s="89" t="s">
+      <c r="C32" s="76">
+        <v>0</v>
+      </c>
+      <c r="D32" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="76">
+        <v>0</v>
+      </c>
+      <c r="F32" s="76">
+        <v>1</v>
+      </c>
+      <c r="G32" s="76" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="91" t="s">
+      <c r="A33" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="93">
-        <v>0</v>
-      </c>
-      <c r="D33" s="94">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="93">
-        <v>0</v>
-      </c>
-      <c r="F33" s="93">
-        <v>1</v>
-      </c>
-      <c r="G33" s="93" t="s">
+      <c r="C33" s="80">
+        <v>0</v>
+      </c>
+      <c r="D33" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="80">
+        <v>0</v>
+      </c>
+      <c r="F33" s="80">
+        <v>1</v>
+      </c>
+      <c r="G33" s="80" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="88" t="s">
+      <c r="B34" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="89">
-        <v>0</v>
-      </c>
-      <c r="D34" s="95">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="89">
-        <v>0</v>
-      </c>
-      <c r="F34" s="89">
-        <v>1</v>
-      </c>
-      <c r="G34" s="89" t="s">
+      <c r="C34" s="76">
+        <v>0</v>
+      </c>
+      <c r="D34" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="76">
+        <v>0</v>
+      </c>
+      <c r="F34" s="76">
+        <v>1</v>
+      </c>
+      <c r="G34" s="76" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="91" t="s">
+      <c r="A35" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="92" t="s">
+      <c r="B35" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="93">
-        <v>0</v>
-      </c>
-      <c r="D35" s="94">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="93">
-        <v>0</v>
-      </c>
-      <c r="F35" s="93">
-        <v>1</v>
-      </c>
-      <c r="G35" s="93" t="s">
+      <c r="C35" s="80">
+        <v>0</v>
+      </c>
+      <c r="D35" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="80">
+        <v>0</v>
+      </c>
+      <c r="F35" s="80">
+        <v>1</v>
+      </c>
+      <c r="G35" s="80" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="87" t="s">
+      <c r="A36" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="88" t="s">
+      <c r="B36" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="89">
-        <v>0</v>
-      </c>
-      <c r="D36" s="95">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="89">
-        <v>0</v>
-      </c>
-      <c r="F36" s="89">
-        <v>1</v>
-      </c>
-      <c r="G36" s="89" t="s">
+      <c r="C36" s="76">
+        <v>0</v>
+      </c>
+      <c r="D36" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="76">
+        <v>0</v>
+      </c>
+      <c r="F36" s="76">
+        <v>1</v>
+      </c>
+      <c r="G36" s="76" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="34" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="113" t="s">
+      <c r="A37" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="114" t="s">
+      <c r="B37" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="115">
-        <v>0</v>
-      </c>
-      <c r="D37" s="116">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="115">
-        <v>0</v>
-      </c>
-      <c r="F37" s="115">
-        <v>1</v>
-      </c>
-      <c r="G37" s="115" t="s">
+      <c r="C37" s="102">
+        <v>0</v>
+      </c>
+      <c r="D37" s="103">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="102">
+        <v>0</v>
+      </c>
+      <c r="F37" s="102">
+        <v>1</v>
+      </c>
+      <c r="G37" s="102" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="50" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08090FAB-59A7-2341-9E58-CF25F3A3E3D3}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="13.1640625" style="71" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="71" customWidth="1"/>
+    <col min="7" max="7" width="23" style="71" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="72" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="73"/>
+      <c r="B1" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="76">
+        <v>0</v>
+      </c>
+      <c r="D2" s="77">
+        <f>C2/858</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="76">
+        <v>13</v>
+      </c>
+      <c r="F2" s="76">
+        <v>84</v>
+      </c>
+      <c r="G2" s="76" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="80">
+        <v>26</v>
+      </c>
+      <c r="D3" s="81">
+        <f t="shared" ref="D3:D37" si="0">C3/858</f>
+        <v>3.0303030303030304E-2</v>
+      </c>
+      <c r="E3" s="80">
+        <v>1</v>
+      </c>
+      <c r="F3" s="80">
+        <v>28</v>
+      </c>
+      <c r="G3" s="80" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="76">
+        <v>7</v>
+      </c>
+      <c r="D4" s="82">
+        <f t="shared" si="0"/>
+        <v>8.1585081585081581E-3</v>
+      </c>
+      <c r="E4" s="76">
+        <v>10</v>
+      </c>
+      <c r="F4" s="76">
+        <v>32</v>
+      </c>
+      <c r="G4" s="76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="80">
+        <v>56</v>
+      </c>
+      <c r="D5" s="81">
+        <f t="shared" si="0"/>
+        <v>6.5268065268065265E-2</v>
+      </c>
+      <c r="E5" s="80">
+        <v>0</v>
+      </c>
+      <c r="F5" s="80">
+        <v>11</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="85">
+        <v>13</v>
+      </c>
+      <c r="D6" s="86">
+        <f t="shared" si="0"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="E6" s="85">
+        <v>0</v>
+      </c>
+      <c r="F6" s="85">
+        <v>1</v>
+      </c>
+      <c r="G6" s="85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="76">
+        <v>13</v>
+      </c>
+      <c r="D7" s="82">
+        <f t="shared" si="0"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="E7" s="76">
+        <v>0</v>
+      </c>
+      <c r="F7" s="76">
+        <v>37</v>
+      </c>
+      <c r="G7" s="76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="76">
+        <v>13</v>
+      </c>
+      <c r="D8" s="82">
+        <f t="shared" si="0"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="E8" s="76">
+        <v>0</v>
+      </c>
+      <c r="F8" s="76">
+        <v>37</v>
+      </c>
+      <c r="G8" s="76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="39" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="87" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="89">
+        <v>108</v>
+      </c>
+      <c r="D9" s="90">
+        <f t="shared" si="0"/>
+        <v>0.12587412587412589</v>
+      </c>
+      <c r="E9" s="89">
+        <v>0</v>
+      </c>
+      <c r="F9" s="89">
+        <v>1</v>
+      </c>
+      <c r="G9" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="14" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="91" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="93">
+        <v>108</v>
+      </c>
+      <c r="D10" s="94">
+        <f t="shared" si="0"/>
+        <v>0.12587412587412589</v>
+      </c>
+      <c r="E10" s="93">
+        <v>0</v>
+      </c>
+      <c r="F10" s="93">
+        <v>30</v>
+      </c>
+      <c r="G10" s="93" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="40" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="85">
+        <v>117</v>
+      </c>
+      <c r="D11" s="86">
+        <f t="shared" si="0"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="E11" s="85">
+        <v>0</v>
+      </c>
+      <c r="F11" s="85">
+        <v>1</v>
+      </c>
+      <c r="G11" s="85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="76">
+        <v>117</v>
+      </c>
+      <c r="D12" s="82">
+        <f t="shared" si="0"/>
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="E12" s="76">
+        <v>0</v>
+      </c>
+      <c r="F12" s="76">
+        <v>19</v>
+      </c>
+      <c r="G12" s="76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="40" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="97">
+        <v>105</v>
+      </c>
+      <c r="D13" s="98">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E13" s="97">
+        <v>0</v>
+      </c>
+      <c r="F13" s="97">
+        <v>1</v>
+      </c>
+      <c r="G13" s="97" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="97">
+        <v>105</v>
+      </c>
+      <c r="D14" s="98">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E14" s="97">
+        <v>0</v>
+      </c>
+      <c r="F14" s="97">
+        <v>4</v>
+      </c>
+      <c r="G14" s="97" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="80">
+        <v>105</v>
+      </c>
+      <c r="D15" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E15" s="80">
+        <v>0</v>
+      </c>
+      <c r="F15" s="80">
+        <v>1</v>
+      </c>
+      <c r="G15" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="80">
+        <v>105</v>
+      </c>
+      <c r="D16" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E16" s="80">
+        <v>0</v>
+      </c>
+      <c r="F16" s="80">
+        <v>1</v>
+      </c>
+      <c r="G16" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="80">
+        <v>105</v>
+      </c>
+      <c r="D17" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E17" s="80">
+        <v>0</v>
+      </c>
+      <c r="F17" s="80">
+        <v>1</v>
+      </c>
+      <c r="G17" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="80">
+        <v>105</v>
+      </c>
+      <c r="D18" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E18" s="80">
+        <v>0</v>
+      </c>
+      <c r="F18" s="80">
+        <v>1</v>
+      </c>
+      <c r="G18" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="80">
+        <v>105</v>
+      </c>
+      <c r="D19" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E19" s="80">
+        <v>0</v>
+      </c>
+      <c r="F19" s="80">
+        <v>1</v>
+      </c>
+      <c r="G19" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="80">
+        <v>105</v>
+      </c>
+      <c r="D20" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E20" s="80">
+        <v>0</v>
+      </c>
+      <c r="F20" s="80">
+        <v>1</v>
+      </c>
+      <c r="G20" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="80">
+        <v>105</v>
+      </c>
+      <c r="D21" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E21" s="80">
+        <v>0</v>
+      </c>
+      <c r="F21" s="80">
+        <v>1</v>
+      </c>
+      <c r="G21" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="80">
+        <v>105</v>
+      </c>
+      <c r="D22" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E22" s="80">
+        <v>0</v>
+      </c>
+      <c r="F22" s="80">
+        <v>1</v>
+      </c>
+      <c r="G22" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="80">
+        <v>105</v>
+      </c>
+      <c r="D23" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E23" s="80">
+        <v>0</v>
+      </c>
+      <c r="F23" s="80">
+        <v>1</v>
+      </c>
+      <c r="G23" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="80">
+        <v>105</v>
+      </c>
+      <c r="D24" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E24" s="80">
+        <v>0</v>
+      </c>
+      <c r="F24" s="80">
+        <v>1</v>
+      </c>
+      <c r="G24" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="80">
+        <v>105</v>
+      </c>
+      <c r="D25" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E25" s="80">
+        <v>0</v>
+      </c>
+      <c r="F25" s="80">
+        <v>1</v>
+      </c>
+      <c r="G25" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="80">
+        <v>105</v>
+      </c>
+      <c r="D26" s="81">
+        <f t="shared" si="0"/>
+        <v>0.12237762237762238</v>
+      </c>
+      <c r="E26" s="80">
+        <v>0</v>
+      </c>
+      <c r="F26" s="80">
+        <v>1</v>
+      </c>
+      <c r="G26" s="89" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="74" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="76">
+        <v>0</v>
+      </c>
+      <c r="D27" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="76">
+        <v>0</v>
+      </c>
+      <c r="F27" s="76">
+        <v>3</v>
+      </c>
+      <c r="G27" s="76" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="80">
+        <v>787</v>
+      </c>
+      <c r="D28" s="99">
+        <f t="shared" si="0"/>
+        <v>0.91724941724941722</v>
+      </c>
+      <c r="E28" s="80">
+        <v>1</v>
+      </c>
+      <c r="F28" s="80">
+        <v>22</v>
+      </c>
+      <c r="G28" s="80" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="80">
+        <v>787</v>
+      </c>
+      <c r="D29" s="99">
+        <f t="shared" si="0"/>
+        <v>0.91724941724941722</v>
+      </c>
+      <c r="E29" s="80">
+        <v>1</v>
+      </c>
+      <c r="F29" s="80">
+        <v>22</v>
+      </c>
+      <c r="G29" s="80" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="76">
+        <v>0</v>
+      </c>
+      <c r="D30" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="76">
+        <v>0</v>
+      </c>
+      <c r="F30" s="76">
+        <v>1</v>
+      </c>
+      <c r="G30" s="76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="80">
+        <v>0</v>
+      </c>
+      <c r="D31" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="80">
+        <v>0</v>
+      </c>
+      <c r="F31" s="80">
+        <v>1</v>
+      </c>
+      <c r="G31" s="80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="76">
+        <v>0</v>
+      </c>
+      <c r="D32" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="76">
+        <v>0</v>
+      </c>
+      <c r="F32" s="76">
+        <v>1</v>
+      </c>
+      <c r="G32" s="76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="80">
+        <v>0</v>
+      </c>
+      <c r="D33" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="80">
+        <v>0</v>
+      </c>
+      <c r="F33" s="80">
+        <v>1</v>
+      </c>
+      <c r="G33" s="80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="76">
+        <v>0</v>
+      </c>
+      <c r="D34" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="76">
+        <v>0</v>
+      </c>
+      <c r="F34" s="76">
+        <v>1</v>
+      </c>
+      <c r="G34" s="76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="80">
+        <v>0</v>
+      </c>
+      <c r="D35" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="80">
+        <v>0</v>
+      </c>
+      <c r="F35" s="80">
+        <v>1</v>
+      </c>
+      <c r="G35" s="80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="76">
+        <v>0</v>
+      </c>
+      <c r="D36" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="76">
+        <v>0</v>
+      </c>
+      <c r="F36" s="76">
+        <v>1</v>
+      </c>
+      <c r="G36" s="76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="34" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="102">
+        <v>0</v>
+      </c>
+      <c r="D37" s="103">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="102">
+        <v>0</v>
+      </c>
+      <c r="F37" s="102">
+        <v>1</v>
+      </c>
+      <c r="G37" s="102" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>